<commit_message>
[#7645] change excel layout
</commit_message>
<xml_diff>
--- a/storage/app/excel/contact_book_0.xlsx
+++ b/storage/app/excel/contact_book_0.xlsx
@@ -144,10 +144,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -165,6 +165,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -173,7 +181,7 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -195,38 +203,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -240,17 +218,31 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -264,7 +256,7 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -281,9 +273,9 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -295,15 +287,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -366,13 +366,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -384,49 +426,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -438,49 +468,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -498,25 +486,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -528,7 +498,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -540,13 +528,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -678,6 +678,45 @@
       <right/>
       <top/>
       <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -698,21 +737,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -720,30 +744,6 @@
       </top>
       <bottom style="double">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -766,8 +766,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -776,13 +776,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -794,134 +794,134 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="15" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="18" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -978,6 +978,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1360,11 +1363,14 @@
   <sheetPr/>
   <dimension ref="A1:ACU79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="E58" sqref="E58:G59"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="15.4285714285714" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:775">
       <c r="A1" s="1"/>
@@ -7616,18 +7622,18 @@
       </c>
       <c r="L9" s="6"/>
       <c r="M9" s="6"/>
-      <c r="N9" s="19"/>
-      <c r="O9" s="20"/>
-      <c r="P9" s="20"/>
-      <c r="Q9" s="20"/>
-      <c r="R9" s="20"/>
-      <c r="S9" s="20"/>
-      <c r="T9" s="20"/>
-      <c r="U9" s="20"/>
-      <c r="V9" s="20"/>
-      <c r="W9" s="20"/>
-      <c r="X9" s="20"/>
-      <c r="Y9" s="33"/>
+      <c r="N9" s="20"/>
+      <c r="O9" s="21"/>
+      <c r="P9" s="21"/>
+      <c r="Q9" s="21"/>
+      <c r="R9" s="21"/>
+      <c r="S9" s="21"/>
+      <c r="T9" s="21"/>
+      <c r="U9" s="21"/>
+      <c r="V9" s="21"/>
+      <c r="W9" s="21"/>
+      <c r="X9" s="21"/>
+      <c r="Y9" s="34"/>
       <c r="Z9" s="1"/>
       <c r="AA9" s="1"/>
       <c r="AB9" s="1"/>
@@ -9171,27 +9177,27 @@
       <c r="H11" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="I11" s="21"/>
-      <c r="J11" s="22"/>
+      <c r="I11" s="22"/>
+      <c r="J11" s="23"/>
       <c r="K11" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="L11" s="21"/>
-      <c r="M11" s="21"/>
-      <c r="N11" s="22"/>
+      <c r="L11" s="22"/>
+      <c r="M11" s="22"/>
+      <c r="N11" s="23"/>
       <c r="O11" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="P11" s="21"/>
-      <c r="Q11" s="21"/>
-      <c r="R11" s="21"/>
-      <c r="S11" s="21"/>
-      <c r="T11" s="21"/>
-      <c r="U11" s="21"/>
-      <c r="V11" s="21"/>
-      <c r="W11" s="21"/>
-      <c r="X11" s="21"/>
-      <c r="Y11" s="22"/>
+      <c r="P11" s="22"/>
+      <c r="Q11" s="22"/>
+      <c r="R11" s="22"/>
+      <c r="S11" s="22"/>
+      <c r="T11" s="22"/>
+      <c r="U11" s="22"/>
+      <c r="V11" s="22"/>
+      <c r="W11" s="22"/>
+      <c r="X11" s="22"/>
+      <c r="Y11" s="23"/>
       <c r="Z11" s="1"/>
       <c r="AA11" s="1"/>
       <c r="AB11" s="1"/>
@@ -9954,23 +9960,23 @@
       <c r="F12" s="11"/>
       <c r="G12" s="11"/>
       <c r="H12" s="12"/>
-      <c r="I12" s="23"/>
-      <c r="J12" s="24"/>
+      <c r="I12" s="24"/>
+      <c r="J12" s="25"/>
       <c r="K12" s="12"/>
-      <c r="L12" s="23"/>
-      <c r="M12" s="23"/>
-      <c r="N12" s="24"/>
+      <c r="L12" s="24"/>
+      <c r="M12" s="24"/>
+      <c r="N12" s="25"/>
       <c r="O12" s="12"/>
-      <c r="P12" s="23"/>
-      <c r="Q12" s="23"/>
-      <c r="R12" s="23"/>
-      <c r="S12" s="23"/>
-      <c r="T12" s="23"/>
-      <c r="U12" s="23"/>
-      <c r="V12" s="23"/>
-      <c r="W12" s="23"/>
-      <c r="X12" s="23"/>
-      <c r="Y12" s="24"/>
+      <c r="P12" s="24"/>
+      <c r="Q12" s="24"/>
+      <c r="R12" s="24"/>
+      <c r="S12" s="24"/>
+      <c r="T12" s="24"/>
+      <c r="U12" s="24"/>
+      <c r="V12" s="24"/>
+      <c r="W12" s="24"/>
+      <c r="X12" s="24"/>
+      <c r="Y12" s="25"/>
       <c r="Z12" s="1"/>
       <c r="AA12" s="1"/>
       <c r="AB12" s="1"/>
@@ -10731,23 +10737,23 @@
       <c r="F13" s="13"/>
       <c r="G13" s="13"/>
       <c r="H13" s="14"/>
-      <c r="I13" s="25"/>
-      <c r="J13" s="26"/>
+      <c r="I13" s="26"/>
+      <c r="J13" s="27"/>
       <c r="K13" s="14"/>
-      <c r="L13" s="25"/>
-      <c r="M13" s="25"/>
-      <c r="N13" s="26"/>
+      <c r="L13" s="26"/>
+      <c r="M13" s="26"/>
+      <c r="N13" s="27"/>
       <c r="O13" s="14"/>
-      <c r="P13" s="25"/>
-      <c r="Q13" s="25"/>
-      <c r="R13" s="25"/>
-      <c r="S13" s="25"/>
-      <c r="T13" s="25"/>
-      <c r="U13" s="25"/>
-      <c r="V13" s="25"/>
-      <c r="W13" s="25"/>
-      <c r="X13" s="25"/>
-      <c r="Y13" s="26"/>
+      <c r="P13" s="26"/>
+      <c r="Q13" s="26"/>
+      <c r="R13" s="26"/>
+      <c r="S13" s="26"/>
+      <c r="T13" s="26"/>
+      <c r="U13" s="26"/>
+      <c r="V13" s="26"/>
+      <c r="W13" s="26"/>
+      <c r="X13" s="26"/>
+      <c r="Y13" s="27"/>
       <c r="Z13" s="1"/>
       <c r="AA13" s="1"/>
       <c r="AB13" s="1"/>
@@ -11510,23 +11516,23 @@
       <c r="F14" s="11"/>
       <c r="G14" s="11"/>
       <c r="H14" s="12"/>
-      <c r="I14" s="23"/>
-      <c r="J14" s="24"/>
+      <c r="I14" s="24"/>
+      <c r="J14" s="25"/>
       <c r="K14" s="12"/>
-      <c r="L14" s="23"/>
-      <c r="M14" s="23"/>
-      <c r="N14" s="24"/>
+      <c r="L14" s="24"/>
+      <c r="M14" s="24"/>
+      <c r="N14" s="25"/>
       <c r="O14" s="12"/>
-      <c r="P14" s="23"/>
-      <c r="Q14" s="23"/>
-      <c r="R14" s="23"/>
-      <c r="S14" s="23"/>
-      <c r="T14" s="23"/>
-      <c r="U14" s="23"/>
-      <c r="V14" s="23"/>
-      <c r="W14" s="23"/>
-      <c r="X14" s="23"/>
-      <c r="Y14" s="24"/>
+      <c r="P14" s="24"/>
+      <c r="Q14" s="24"/>
+      <c r="R14" s="24"/>
+      <c r="S14" s="24"/>
+      <c r="T14" s="24"/>
+      <c r="U14" s="24"/>
+      <c r="V14" s="24"/>
+      <c r="W14" s="24"/>
+      <c r="X14" s="24"/>
+      <c r="Y14" s="25"/>
       <c r="Z14" s="1"/>
       <c r="AA14" s="1"/>
       <c r="AB14" s="1"/>
@@ -12287,23 +12293,23 @@
       <c r="F15" s="13"/>
       <c r="G15" s="13"/>
       <c r="H15" s="14"/>
-      <c r="I15" s="25"/>
-      <c r="J15" s="26"/>
+      <c r="I15" s="26"/>
+      <c r="J15" s="27"/>
       <c r="K15" s="14"/>
-      <c r="L15" s="25"/>
-      <c r="M15" s="25"/>
-      <c r="N15" s="26"/>
+      <c r="L15" s="26"/>
+      <c r="M15" s="26"/>
+      <c r="N15" s="27"/>
       <c r="O15" s="14"/>
-      <c r="P15" s="25"/>
-      <c r="Q15" s="25"/>
-      <c r="R15" s="25"/>
-      <c r="S15" s="25"/>
-      <c r="T15" s="25"/>
-      <c r="U15" s="25"/>
-      <c r="V15" s="25"/>
-      <c r="W15" s="25"/>
-      <c r="X15" s="25"/>
-      <c r="Y15" s="26"/>
+      <c r="P15" s="26"/>
+      <c r="Q15" s="26"/>
+      <c r="R15" s="26"/>
+      <c r="S15" s="26"/>
+      <c r="T15" s="26"/>
+      <c r="U15" s="26"/>
+      <c r="V15" s="26"/>
+      <c r="W15" s="26"/>
+      <c r="X15" s="26"/>
+      <c r="Y15" s="27"/>
       <c r="Z15" s="1"/>
       <c r="AA15" s="1"/>
       <c r="AB15" s="1"/>
@@ -13066,23 +13072,23 @@
       <c r="F16" s="11"/>
       <c r="G16" s="11"/>
       <c r="H16" s="12"/>
-      <c r="I16" s="23"/>
-      <c r="J16" s="24"/>
+      <c r="I16" s="24"/>
+      <c r="J16" s="25"/>
       <c r="K16" s="12"/>
-      <c r="L16" s="23"/>
-      <c r="M16" s="23"/>
-      <c r="N16" s="24"/>
+      <c r="L16" s="24"/>
+      <c r="M16" s="24"/>
+      <c r="N16" s="25"/>
       <c r="O16" s="12"/>
-      <c r="P16" s="23"/>
-      <c r="Q16" s="23"/>
-      <c r="R16" s="23"/>
-      <c r="S16" s="23"/>
-      <c r="T16" s="23"/>
-      <c r="U16" s="23"/>
-      <c r="V16" s="23"/>
-      <c r="W16" s="23"/>
-      <c r="X16" s="23"/>
-      <c r="Y16" s="24"/>
+      <c r="P16" s="24"/>
+      <c r="Q16" s="24"/>
+      <c r="R16" s="24"/>
+      <c r="S16" s="24"/>
+      <c r="T16" s="24"/>
+      <c r="U16" s="24"/>
+      <c r="V16" s="24"/>
+      <c r="W16" s="24"/>
+      <c r="X16" s="24"/>
+      <c r="Y16" s="25"/>
       <c r="Z16" s="1"/>
       <c r="AA16" s="1"/>
       <c r="AB16" s="1"/>
@@ -13843,23 +13849,23 @@
       <c r="F17" s="13"/>
       <c r="G17" s="13"/>
       <c r="H17" s="14"/>
-      <c r="I17" s="25"/>
-      <c r="J17" s="26"/>
+      <c r="I17" s="26"/>
+      <c r="J17" s="27"/>
       <c r="K17" s="14"/>
-      <c r="L17" s="25"/>
-      <c r="M17" s="25"/>
-      <c r="N17" s="26"/>
+      <c r="L17" s="26"/>
+      <c r="M17" s="26"/>
+      <c r="N17" s="27"/>
       <c r="O17" s="14"/>
-      <c r="P17" s="25"/>
-      <c r="Q17" s="25"/>
-      <c r="R17" s="25"/>
-      <c r="S17" s="25"/>
-      <c r="T17" s="25"/>
-      <c r="U17" s="25"/>
-      <c r="V17" s="25"/>
-      <c r="W17" s="25"/>
-      <c r="X17" s="25"/>
-      <c r="Y17" s="26"/>
+      <c r="P17" s="26"/>
+      <c r="Q17" s="26"/>
+      <c r="R17" s="26"/>
+      <c r="S17" s="26"/>
+      <c r="T17" s="26"/>
+      <c r="U17" s="26"/>
+      <c r="V17" s="26"/>
+      <c r="W17" s="26"/>
+      <c r="X17" s="26"/>
+      <c r="Y17" s="27"/>
       <c r="Z17" s="1"/>
       <c r="AA17" s="1"/>
       <c r="AB17" s="1"/>
@@ -14622,23 +14628,23 @@
       <c r="F18" s="11"/>
       <c r="G18" s="11"/>
       <c r="H18" s="12"/>
-      <c r="I18" s="23"/>
-      <c r="J18" s="24"/>
+      <c r="I18" s="24"/>
+      <c r="J18" s="25"/>
       <c r="K18" s="12"/>
-      <c r="L18" s="23"/>
-      <c r="M18" s="23"/>
-      <c r="N18" s="24"/>
+      <c r="L18" s="24"/>
+      <c r="M18" s="24"/>
+      <c r="N18" s="25"/>
       <c r="O18" s="12"/>
-      <c r="P18" s="23"/>
-      <c r="Q18" s="23"/>
-      <c r="R18" s="23"/>
-      <c r="S18" s="23"/>
-      <c r="T18" s="23"/>
-      <c r="U18" s="23"/>
-      <c r="V18" s="23"/>
-      <c r="W18" s="23"/>
-      <c r="X18" s="23"/>
-      <c r="Y18" s="24"/>
+      <c r="P18" s="24"/>
+      <c r="Q18" s="24"/>
+      <c r="R18" s="24"/>
+      <c r="S18" s="24"/>
+      <c r="T18" s="24"/>
+      <c r="U18" s="24"/>
+      <c r="V18" s="24"/>
+      <c r="W18" s="24"/>
+      <c r="X18" s="24"/>
+      <c r="Y18" s="25"/>
       <c r="Z18" s="1"/>
       <c r="AA18" s="1"/>
       <c r="AB18" s="1"/>
@@ -15399,23 +15405,23 @@
       <c r="F19" s="13"/>
       <c r="G19" s="13"/>
       <c r="H19" s="14"/>
-      <c r="I19" s="25"/>
-      <c r="J19" s="26"/>
+      <c r="I19" s="26"/>
+      <c r="J19" s="27"/>
       <c r="K19" s="14"/>
-      <c r="L19" s="25"/>
-      <c r="M19" s="25"/>
-      <c r="N19" s="26"/>
+      <c r="L19" s="26"/>
+      <c r="M19" s="26"/>
+      <c r="N19" s="27"/>
       <c r="O19" s="14"/>
-      <c r="P19" s="25"/>
-      <c r="Q19" s="25"/>
-      <c r="R19" s="25"/>
-      <c r="S19" s="25"/>
-      <c r="T19" s="25"/>
-      <c r="U19" s="25"/>
-      <c r="V19" s="25"/>
-      <c r="W19" s="25"/>
-      <c r="X19" s="25"/>
-      <c r="Y19" s="26"/>
+      <c r="P19" s="26"/>
+      <c r="Q19" s="26"/>
+      <c r="R19" s="26"/>
+      <c r="S19" s="26"/>
+      <c r="T19" s="26"/>
+      <c r="U19" s="26"/>
+      <c r="V19" s="26"/>
+      <c r="W19" s="26"/>
+      <c r="X19" s="26"/>
+      <c r="Y19" s="27"/>
       <c r="Z19" s="1"/>
       <c r="AA19" s="1"/>
       <c r="AB19" s="1"/>
@@ -16178,23 +16184,23 @@
       <c r="F20" s="11"/>
       <c r="G20" s="11"/>
       <c r="H20" s="12"/>
-      <c r="I20" s="23"/>
-      <c r="J20" s="24"/>
+      <c r="I20" s="24"/>
+      <c r="J20" s="25"/>
       <c r="K20" s="12"/>
-      <c r="L20" s="23"/>
-      <c r="M20" s="23"/>
-      <c r="N20" s="24"/>
+      <c r="L20" s="24"/>
+      <c r="M20" s="24"/>
+      <c r="N20" s="25"/>
       <c r="O20" s="12"/>
-      <c r="P20" s="23"/>
-      <c r="Q20" s="23"/>
-      <c r="R20" s="23"/>
-      <c r="S20" s="23"/>
-      <c r="T20" s="23"/>
-      <c r="U20" s="23"/>
-      <c r="V20" s="23"/>
-      <c r="W20" s="23"/>
-      <c r="X20" s="23"/>
-      <c r="Y20" s="24"/>
+      <c r="P20" s="24"/>
+      <c r="Q20" s="24"/>
+      <c r="R20" s="24"/>
+      <c r="S20" s="24"/>
+      <c r="T20" s="24"/>
+      <c r="U20" s="24"/>
+      <c r="V20" s="24"/>
+      <c r="W20" s="24"/>
+      <c r="X20" s="24"/>
+      <c r="Y20" s="25"/>
       <c r="Z20" s="1"/>
       <c r="AA20" s="1"/>
       <c r="AB20" s="1"/>
@@ -16955,23 +16961,23 @@
       <c r="F21" s="13"/>
       <c r="G21" s="13"/>
       <c r="H21" s="14"/>
-      <c r="I21" s="25"/>
-      <c r="J21" s="26"/>
+      <c r="I21" s="26"/>
+      <c r="J21" s="27"/>
       <c r="K21" s="14"/>
-      <c r="L21" s="25"/>
-      <c r="M21" s="25"/>
-      <c r="N21" s="26"/>
+      <c r="L21" s="26"/>
+      <c r="M21" s="26"/>
+      <c r="N21" s="27"/>
       <c r="O21" s="14"/>
-      <c r="P21" s="25"/>
-      <c r="Q21" s="25"/>
-      <c r="R21" s="25"/>
-      <c r="S21" s="25"/>
-      <c r="T21" s="25"/>
-      <c r="U21" s="25"/>
-      <c r="V21" s="25"/>
-      <c r="W21" s="25"/>
-      <c r="X21" s="25"/>
-      <c r="Y21" s="26"/>
+      <c r="P21" s="26"/>
+      <c r="Q21" s="26"/>
+      <c r="R21" s="26"/>
+      <c r="S21" s="26"/>
+      <c r="T21" s="26"/>
+      <c r="U21" s="26"/>
+      <c r="V21" s="26"/>
+      <c r="W21" s="26"/>
+      <c r="X21" s="26"/>
+      <c r="Y21" s="27"/>
       <c r="Z21" s="1"/>
       <c r="AA21" s="1"/>
       <c r="AB21" s="1"/>
@@ -17734,23 +17740,23 @@
       <c r="F22" s="11"/>
       <c r="G22" s="11"/>
       <c r="H22" s="12"/>
-      <c r="I22" s="23"/>
-      <c r="J22" s="24"/>
+      <c r="I22" s="24"/>
+      <c r="J22" s="25"/>
       <c r="K22" s="12"/>
-      <c r="L22" s="23"/>
-      <c r="M22" s="23"/>
-      <c r="N22" s="24"/>
+      <c r="L22" s="24"/>
+      <c r="M22" s="24"/>
+      <c r="N22" s="25"/>
       <c r="O22" s="12"/>
-      <c r="P22" s="23"/>
-      <c r="Q22" s="23"/>
-      <c r="R22" s="23"/>
-      <c r="S22" s="23"/>
-      <c r="T22" s="23"/>
-      <c r="U22" s="23"/>
-      <c r="V22" s="23"/>
-      <c r="W22" s="23"/>
-      <c r="X22" s="23"/>
-      <c r="Y22" s="24"/>
+      <c r="P22" s="24"/>
+      <c r="Q22" s="24"/>
+      <c r="R22" s="24"/>
+      <c r="S22" s="24"/>
+      <c r="T22" s="24"/>
+      <c r="U22" s="24"/>
+      <c r="V22" s="24"/>
+      <c r="W22" s="24"/>
+      <c r="X22" s="24"/>
+      <c r="Y22" s="25"/>
       <c r="Z22" s="1"/>
       <c r="AA22" s="1"/>
       <c r="AB22" s="1"/>
@@ -18511,23 +18517,23 @@
       <c r="F23" s="13"/>
       <c r="G23" s="13"/>
       <c r="H23" s="14"/>
-      <c r="I23" s="25"/>
-      <c r="J23" s="26"/>
+      <c r="I23" s="26"/>
+      <c r="J23" s="27"/>
       <c r="K23" s="14"/>
-      <c r="L23" s="25"/>
-      <c r="M23" s="25"/>
-      <c r="N23" s="26"/>
+      <c r="L23" s="26"/>
+      <c r="M23" s="26"/>
+      <c r="N23" s="27"/>
       <c r="O23" s="14"/>
-      <c r="P23" s="25"/>
-      <c r="Q23" s="25"/>
-      <c r="R23" s="25"/>
-      <c r="S23" s="25"/>
-      <c r="T23" s="25"/>
-      <c r="U23" s="25"/>
-      <c r="V23" s="25"/>
-      <c r="W23" s="25"/>
-      <c r="X23" s="25"/>
-      <c r="Y23" s="26"/>
+      <c r="P23" s="26"/>
+      <c r="Q23" s="26"/>
+      <c r="R23" s="26"/>
+      <c r="S23" s="26"/>
+      <c r="T23" s="26"/>
+      <c r="U23" s="26"/>
+      <c r="V23" s="26"/>
+      <c r="W23" s="26"/>
+      <c r="X23" s="26"/>
+      <c r="Y23" s="27"/>
       <c r="Z23" s="1"/>
       <c r="AA23" s="1"/>
       <c r="AB23" s="1"/>
@@ -19290,23 +19296,23 @@
       <c r="F24" s="11"/>
       <c r="G24" s="11"/>
       <c r="H24" s="12"/>
-      <c r="I24" s="23"/>
-      <c r="J24" s="24"/>
+      <c r="I24" s="24"/>
+      <c r="J24" s="25"/>
       <c r="K24" s="12"/>
-      <c r="L24" s="23"/>
-      <c r="M24" s="23"/>
-      <c r="N24" s="24"/>
+      <c r="L24" s="24"/>
+      <c r="M24" s="24"/>
+      <c r="N24" s="25"/>
       <c r="O24" s="12"/>
-      <c r="P24" s="23"/>
-      <c r="Q24" s="23"/>
-      <c r="R24" s="23"/>
-      <c r="S24" s="23"/>
-      <c r="T24" s="23"/>
-      <c r="U24" s="23"/>
-      <c r="V24" s="23"/>
-      <c r="W24" s="23"/>
-      <c r="X24" s="23"/>
-      <c r="Y24" s="24"/>
+      <c r="P24" s="24"/>
+      <c r="Q24" s="24"/>
+      <c r="R24" s="24"/>
+      <c r="S24" s="24"/>
+      <c r="T24" s="24"/>
+      <c r="U24" s="24"/>
+      <c r="V24" s="24"/>
+      <c r="W24" s="24"/>
+      <c r="X24" s="24"/>
+      <c r="Y24" s="25"/>
       <c r="Z24" s="1"/>
       <c r="AA24" s="1"/>
       <c r="AB24" s="1"/>
@@ -20067,23 +20073,23 @@
       <c r="F25" s="13"/>
       <c r="G25" s="13"/>
       <c r="H25" s="14"/>
-      <c r="I25" s="25"/>
-      <c r="J25" s="26"/>
+      <c r="I25" s="26"/>
+      <c r="J25" s="27"/>
       <c r="K25" s="14"/>
-      <c r="L25" s="25"/>
-      <c r="M25" s="25"/>
-      <c r="N25" s="26"/>
+      <c r="L25" s="26"/>
+      <c r="M25" s="26"/>
+      <c r="N25" s="27"/>
       <c r="O25" s="14"/>
-      <c r="P25" s="25"/>
-      <c r="Q25" s="25"/>
-      <c r="R25" s="25"/>
-      <c r="S25" s="25"/>
-      <c r="T25" s="25"/>
-      <c r="U25" s="25"/>
-      <c r="V25" s="25"/>
-      <c r="W25" s="25"/>
-      <c r="X25" s="25"/>
-      <c r="Y25" s="26"/>
+      <c r="P25" s="26"/>
+      <c r="Q25" s="26"/>
+      <c r="R25" s="26"/>
+      <c r="S25" s="26"/>
+      <c r="T25" s="26"/>
+      <c r="U25" s="26"/>
+      <c r="V25" s="26"/>
+      <c r="W25" s="26"/>
+      <c r="X25" s="26"/>
+      <c r="Y25" s="27"/>
       <c r="Z25" s="1"/>
       <c r="AA25" s="1"/>
       <c r="AB25" s="1"/>
@@ -20846,23 +20852,23 @@
       <c r="F26" s="11"/>
       <c r="G26" s="11"/>
       <c r="H26" s="12"/>
-      <c r="I26" s="23"/>
-      <c r="J26" s="24"/>
+      <c r="I26" s="24"/>
+      <c r="J26" s="25"/>
       <c r="K26" s="12"/>
-      <c r="L26" s="23"/>
-      <c r="M26" s="23"/>
-      <c r="N26" s="24"/>
+      <c r="L26" s="24"/>
+      <c r="M26" s="24"/>
+      <c r="N26" s="25"/>
       <c r="O26" s="12"/>
-      <c r="P26" s="23"/>
-      <c r="Q26" s="23"/>
-      <c r="R26" s="23"/>
-      <c r="S26" s="23"/>
-      <c r="T26" s="23"/>
-      <c r="U26" s="23"/>
-      <c r="V26" s="23"/>
-      <c r="W26" s="23"/>
-      <c r="X26" s="23"/>
-      <c r="Y26" s="24"/>
+      <c r="P26" s="24"/>
+      <c r="Q26" s="24"/>
+      <c r="R26" s="24"/>
+      <c r="S26" s="24"/>
+      <c r="T26" s="24"/>
+      <c r="U26" s="24"/>
+      <c r="V26" s="24"/>
+      <c r="W26" s="24"/>
+      <c r="X26" s="24"/>
+      <c r="Y26" s="25"/>
       <c r="Z26" s="1"/>
       <c r="AA26" s="1"/>
       <c r="AB26" s="1"/>
@@ -21623,23 +21629,23 @@
       <c r="F27" s="13"/>
       <c r="G27" s="13"/>
       <c r="H27" s="14"/>
-      <c r="I27" s="25"/>
-      <c r="J27" s="26"/>
+      <c r="I27" s="26"/>
+      <c r="J27" s="27"/>
       <c r="K27" s="14"/>
-      <c r="L27" s="25"/>
-      <c r="M27" s="25"/>
-      <c r="N27" s="26"/>
+      <c r="L27" s="26"/>
+      <c r="M27" s="26"/>
+      <c r="N27" s="27"/>
       <c r="O27" s="14"/>
-      <c r="P27" s="25"/>
-      <c r="Q27" s="25"/>
-      <c r="R27" s="25"/>
-      <c r="S27" s="25"/>
-      <c r="T27" s="25"/>
-      <c r="U27" s="25"/>
-      <c r="V27" s="25"/>
-      <c r="W27" s="25"/>
-      <c r="X27" s="25"/>
-      <c r="Y27" s="26"/>
+      <c r="P27" s="26"/>
+      <c r="Q27" s="26"/>
+      <c r="R27" s="26"/>
+      <c r="S27" s="26"/>
+      <c r="T27" s="26"/>
+      <c r="U27" s="26"/>
+      <c r="V27" s="26"/>
+      <c r="W27" s="26"/>
+      <c r="X27" s="26"/>
+      <c r="Y27" s="27"/>
       <c r="Z27" s="1"/>
       <c r="AA27" s="1"/>
       <c r="AB27" s="1"/>
@@ -22402,23 +22408,23 @@
       <c r="F28" s="11"/>
       <c r="G28" s="11"/>
       <c r="H28" s="12"/>
-      <c r="I28" s="23"/>
-      <c r="J28" s="24"/>
+      <c r="I28" s="24"/>
+      <c r="J28" s="25"/>
       <c r="K28" s="12"/>
-      <c r="L28" s="23"/>
-      <c r="M28" s="23"/>
-      <c r="N28" s="24"/>
+      <c r="L28" s="24"/>
+      <c r="M28" s="24"/>
+      <c r="N28" s="25"/>
       <c r="O28" s="12"/>
-      <c r="P28" s="23"/>
-      <c r="Q28" s="23"/>
-      <c r="R28" s="23"/>
-      <c r="S28" s="23"/>
-      <c r="T28" s="23"/>
-      <c r="U28" s="23"/>
-      <c r="V28" s="23"/>
-      <c r="W28" s="23"/>
-      <c r="X28" s="23"/>
-      <c r="Y28" s="24"/>
+      <c r="P28" s="24"/>
+      <c r="Q28" s="24"/>
+      <c r="R28" s="24"/>
+      <c r="S28" s="24"/>
+      <c r="T28" s="24"/>
+      <c r="U28" s="24"/>
+      <c r="V28" s="24"/>
+      <c r="W28" s="24"/>
+      <c r="X28" s="24"/>
+      <c r="Y28" s="25"/>
       <c r="Z28" s="1"/>
       <c r="AA28" s="1"/>
       <c r="AB28" s="1"/>
@@ -23179,23 +23185,23 @@
       <c r="F29" s="13"/>
       <c r="G29" s="13"/>
       <c r="H29" s="14"/>
-      <c r="I29" s="25"/>
-      <c r="J29" s="26"/>
+      <c r="I29" s="26"/>
+      <c r="J29" s="27"/>
       <c r="K29" s="14"/>
-      <c r="L29" s="25"/>
-      <c r="M29" s="25"/>
-      <c r="N29" s="26"/>
+      <c r="L29" s="26"/>
+      <c r="M29" s="26"/>
+      <c r="N29" s="27"/>
       <c r="O29" s="14"/>
-      <c r="P29" s="25"/>
-      <c r="Q29" s="25"/>
-      <c r="R29" s="25"/>
-      <c r="S29" s="25"/>
-      <c r="T29" s="25"/>
-      <c r="U29" s="25"/>
-      <c r="V29" s="25"/>
-      <c r="W29" s="25"/>
-      <c r="X29" s="25"/>
-      <c r="Y29" s="26"/>
+      <c r="P29" s="26"/>
+      <c r="Q29" s="26"/>
+      <c r="R29" s="26"/>
+      <c r="S29" s="26"/>
+      <c r="T29" s="26"/>
+      <c r="U29" s="26"/>
+      <c r="V29" s="26"/>
+      <c r="W29" s="26"/>
+      <c r="X29" s="26"/>
+      <c r="Y29" s="27"/>
       <c r="Z29" s="1"/>
       <c r="AA29" s="1"/>
       <c r="AB29" s="1"/>
@@ -23958,23 +23964,23 @@
       <c r="F30" s="11"/>
       <c r="G30" s="11"/>
       <c r="H30" s="12"/>
-      <c r="I30" s="23"/>
-      <c r="J30" s="24"/>
+      <c r="I30" s="24"/>
+      <c r="J30" s="25"/>
       <c r="K30" s="12"/>
-      <c r="L30" s="23"/>
-      <c r="M30" s="23"/>
-      <c r="N30" s="24"/>
+      <c r="L30" s="24"/>
+      <c r="M30" s="24"/>
+      <c r="N30" s="25"/>
       <c r="O30" s="12"/>
-      <c r="P30" s="23"/>
-      <c r="Q30" s="23"/>
-      <c r="R30" s="23"/>
-      <c r="S30" s="23"/>
-      <c r="T30" s="23"/>
-      <c r="U30" s="23"/>
-      <c r="V30" s="23"/>
-      <c r="W30" s="23"/>
-      <c r="X30" s="23"/>
-      <c r="Y30" s="24"/>
+      <c r="P30" s="24"/>
+      <c r="Q30" s="24"/>
+      <c r="R30" s="24"/>
+      <c r="S30" s="24"/>
+      <c r="T30" s="24"/>
+      <c r="U30" s="24"/>
+      <c r="V30" s="24"/>
+      <c r="W30" s="24"/>
+      <c r="X30" s="24"/>
+      <c r="Y30" s="25"/>
       <c r="Z30" s="1"/>
       <c r="AA30" s="1"/>
       <c r="AB30" s="1"/>
@@ -24735,23 +24741,23 @@
       <c r="F31" s="13"/>
       <c r="G31" s="13"/>
       <c r="H31" s="14"/>
-      <c r="I31" s="25"/>
-      <c r="J31" s="26"/>
+      <c r="I31" s="26"/>
+      <c r="J31" s="27"/>
       <c r="K31" s="14"/>
-      <c r="L31" s="25"/>
-      <c r="M31" s="25"/>
-      <c r="N31" s="26"/>
+      <c r="L31" s="26"/>
+      <c r="M31" s="26"/>
+      <c r="N31" s="27"/>
       <c r="O31" s="14"/>
-      <c r="P31" s="25"/>
-      <c r="Q31" s="25"/>
-      <c r="R31" s="25"/>
-      <c r="S31" s="25"/>
-      <c r="T31" s="25"/>
-      <c r="U31" s="25"/>
-      <c r="V31" s="25"/>
-      <c r="W31" s="25"/>
-      <c r="X31" s="25"/>
-      <c r="Y31" s="26"/>
+      <c r="P31" s="26"/>
+      <c r="Q31" s="26"/>
+      <c r="R31" s="26"/>
+      <c r="S31" s="26"/>
+      <c r="T31" s="26"/>
+      <c r="U31" s="26"/>
+      <c r="V31" s="26"/>
+      <c r="W31" s="26"/>
+      <c r="X31" s="26"/>
+      <c r="Y31" s="27"/>
       <c r="Z31" s="1"/>
       <c r="AA31" s="1"/>
       <c r="AB31" s="1"/>
@@ -25514,23 +25520,23 @@
       <c r="F32" s="11"/>
       <c r="G32" s="11"/>
       <c r="H32" s="12"/>
-      <c r="I32" s="23"/>
-      <c r="J32" s="24"/>
+      <c r="I32" s="24"/>
+      <c r="J32" s="25"/>
       <c r="K32" s="12"/>
-      <c r="L32" s="23"/>
-      <c r="M32" s="23"/>
-      <c r="N32" s="24"/>
+      <c r="L32" s="24"/>
+      <c r="M32" s="24"/>
+      <c r="N32" s="25"/>
       <c r="O32" s="12"/>
-      <c r="P32" s="23"/>
-      <c r="Q32" s="23"/>
-      <c r="R32" s="23"/>
-      <c r="S32" s="23"/>
-      <c r="T32" s="23"/>
-      <c r="U32" s="23"/>
-      <c r="V32" s="23"/>
-      <c r="W32" s="23"/>
-      <c r="X32" s="23"/>
-      <c r="Y32" s="24"/>
+      <c r="P32" s="24"/>
+      <c r="Q32" s="24"/>
+      <c r="R32" s="24"/>
+      <c r="S32" s="24"/>
+      <c r="T32" s="24"/>
+      <c r="U32" s="24"/>
+      <c r="V32" s="24"/>
+      <c r="W32" s="24"/>
+      <c r="X32" s="24"/>
+      <c r="Y32" s="25"/>
       <c r="Z32" s="1"/>
       <c r="AA32" s="1"/>
       <c r="AB32" s="1"/>
@@ -26291,23 +26297,23 @@
       <c r="F33" s="13"/>
       <c r="G33" s="13"/>
       <c r="H33" s="14"/>
-      <c r="I33" s="25"/>
-      <c r="J33" s="26"/>
+      <c r="I33" s="26"/>
+      <c r="J33" s="27"/>
       <c r="K33" s="14"/>
-      <c r="L33" s="25"/>
-      <c r="M33" s="25"/>
-      <c r="N33" s="26"/>
+      <c r="L33" s="26"/>
+      <c r="M33" s="26"/>
+      <c r="N33" s="27"/>
       <c r="O33" s="14"/>
-      <c r="P33" s="25"/>
-      <c r="Q33" s="25"/>
-      <c r="R33" s="25"/>
-      <c r="S33" s="25"/>
-      <c r="T33" s="25"/>
-      <c r="U33" s="25"/>
-      <c r="V33" s="25"/>
-      <c r="W33" s="25"/>
-      <c r="X33" s="25"/>
-      <c r="Y33" s="26"/>
+      <c r="P33" s="26"/>
+      <c r="Q33" s="26"/>
+      <c r="R33" s="26"/>
+      <c r="S33" s="26"/>
+      <c r="T33" s="26"/>
+      <c r="U33" s="26"/>
+      <c r="V33" s="26"/>
+      <c r="W33" s="26"/>
+      <c r="X33" s="26"/>
+      <c r="Y33" s="27"/>
       <c r="Z33" s="1"/>
       <c r="AA33" s="1"/>
       <c r="AB33" s="1"/>
@@ -27070,23 +27076,23 @@
       <c r="F34" s="11"/>
       <c r="G34" s="11"/>
       <c r="H34" s="12"/>
-      <c r="I34" s="23"/>
-      <c r="J34" s="24"/>
+      <c r="I34" s="24"/>
+      <c r="J34" s="25"/>
       <c r="K34" s="12"/>
-      <c r="L34" s="23"/>
-      <c r="M34" s="23"/>
-      <c r="N34" s="24"/>
+      <c r="L34" s="24"/>
+      <c r="M34" s="24"/>
+      <c r="N34" s="25"/>
       <c r="O34" s="12"/>
-      <c r="P34" s="23"/>
-      <c r="Q34" s="23"/>
-      <c r="R34" s="23"/>
-      <c r="S34" s="23"/>
-      <c r="T34" s="23"/>
-      <c r="U34" s="23"/>
-      <c r="V34" s="23"/>
-      <c r="W34" s="23"/>
-      <c r="X34" s="23"/>
-      <c r="Y34" s="24"/>
+      <c r="P34" s="24"/>
+      <c r="Q34" s="24"/>
+      <c r="R34" s="24"/>
+      <c r="S34" s="24"/>
+      <c r="T34" s="24"/>
+      <c r="U34" s="24"/>
+      <c r="V34" s="24"/>
+      <c r="W34" s="24"/>
+      <c r="X34" s="24"/>
+      <c r="Y34" s="25"/>
       <c r="Z34" s="1"/>
       <c r="AA34" s="1"/>
       <c r="AB34" s="1"/>
@@ -27847,23 +27853,23 @@
       <c r="F35" s="13"/>
       <c r="G35" s="13"/>
       <c r="H35" s="14"/>
-      <c r="I35" s="25"/>
-      <c r="J35" s="26"/>
+      <c r="I35" s="26"/>
+      <c r="J35" s="27"/>
       <c r="K35" s="14"/>
-      <c r="L35" s="25"/>
-      <c r="M35" s="25"/>
-      <c r="N35" s="26"/>
+      <c r="L35" s="26"/>
+      <c r="M35" s="26"/>
+      <c r="N35" s="27"/>
       <c r="O35" s="14"/>
-      <c r="P35" s="25"/>
-      <c r="Q35" s="25"/>
-      <c r="R35" s="25"/>
-      <c r="S35" s="25"/>
-      <c r="T35" s="25"/>
-      <c r="U35" s="25"/>
-      <c r="V35" s="25"/>
-      <c r="W35" s="25"/>
-      <c r="X35" s="25"/>
-      <c r="Y35" s="26"/>
+      <c r="P35" s="26"/>
+      <c r="Q35" s="26"/>
+      <c r="R35" s="26"/>
+      <c r="S35" s="26"/>
+      <c r="T35" s="26"/>
+      <c r="U35" s="26"/>
+      <c r="V35" s="26"/>
+      <c r="W35" s="26"/>
+      <c r="X35" s="26"/>
+      <c r="Y35" s="27"/>
       <c r="Z35" s="1"/>
       <c r="AA35" s="1"/>
       <c r="AB35" s="1"/>
@@ -28626,23 +28632,23 @@
       <c r="F36" s="11"/>
       <c r="G36" s="11"/>
       <c r="H36" s="12"/>
-      <c r="I36" s="23"/>
-      <c r="J36" s="24"/>
+      <c r="I36" s="24"/>
+      <c r="J36" s="25"/>
       <c r="K36" s="12"/>
-      <c r="L36" s="23"/>
-      <c r="M36" s="23"/>
-      <c r="N36" s="24"/>
+      <c r="L36" s="24"/>
+      <c r="M36" s="24"/>
+      <c r="N36" s="25"/>
       <c r="O36" s="12"/>
-      <c r="P36" s="23"/>
-      <c r="Q36" s="23"/>
-      <c r="R36" s="23"/>
-      <c r="S36" s="23"/>
-      <c r="T36" s="23"/>
-      <c r="U36" s="23"/>
-      <c r="V36" s="23"/>
-      <c r="W36" s="23"/>
-      <c r="X36" s="23"/>
-      <c r="Y36" s="24"/>
+      <c r="P36" s="24"/>
+      <c r="Q36" s="24"/>
+      <c r="R36" s="24"/>
+      <c r="S36" s="24"/>
+      <c r="T36" s="24"/>
+      <c r="U36" s="24"/>
+      <c r="V36" s="24"/>
+      <c r="W36" s="24"/>
+      <c r="X36" s="24"/>
+      <c r="Y36" s="25"/>
       <c r="Z36" s="1"/>
       <c r="AA36" s="1"/>
       <c r="AB36" s="1"/>
@@ -29403,23 +29409,23 @@
       <c r="F37" s="13"/>
       <c r="G37" s="13"/>
       <c r="H37" s="14"/>
-      <c r="I37" s="25"/>
-      <c r="J37" s="26"/>
+      <c r="I37" s="26"/>
+      <c r="J37" s="27"/>
       <c r="K37" s="14"/>
-      <c r="L37" s="25"/>
-      <c r="M37" s="25"/>
-      <c r="N37" s="26"/>
+      <c r="L37" s="26"/>
+      <c r="M37" s="26"/>
+      <c r="N37" s="27"/>
       <c r="O37" s="14"/>
-      <c r="P37" s="25"/>
-      <c r="Q37" s="25"/>
-      <c r="R37" s="25"/>
-      <c r="S37" s="25"/>
-      <c r="T37" s="25"/>
-      <c r="U37" s="25"/>
-      <c r="V37" s="25"/>
-      <c r="W37" s="25"/>
-      <c r="X37" s="25"/>
-      <c r="Y37" s="26"/>
+      <c r="P37" s="26"/>
+      <c r="Q37" s="26"/>
+      <c r="R37" s="26"/>
+      <c r="S37" s="26"/>
+      <c r="T37" s="26"/>
+      <c r="U37" s="26"/>
+      <c r="V37" s="26"/>
+      <c r="W37" s="26"/>
+      <c r="X37" s="26"/>
+      <c r="Y37" s="27"/>
       <c r="Z37" s="1"/>
       <c r="AA37" s="1"/>
       <c r="AB37" s="1"/>
@@ -30182,23 +30188,23 @@
       <c r="F38" s="11"/>
       <c r="G38" s="11"/>
       <c r="H38" s="12"/>
-      <c r="I38" s="23"/>
-      <c r="J38" s="24"/>
+      <c r="I38" s="24"/>
+      <c r="J38" s="25"/>
       <c r="K38" s="12"/>
-      <c r="L38" s="23"/>
-      <c r="M38" s="23"/>
-      <c r="N38" s="24"/>
+      <c r="L38" s="24"/>
+      <c r="M38" s="24"/>
+      <c r="N38" s="25"/>
       <c r="O38" s="12"/>
-      <c r="P38" s="23"/>
-      <c r="Q38" s="23"/>
-      <c r="R38" s="23"/>
-      <c r="S38" s="23"/>
-      <c r="T38" s="23"/>
-      <c r="U38" s="23"/>
-      <c r="V38" s="23"/>
-      <c r="W38" s="23"/>
-      <c r="X38" s="23"/>
-      <c r="Y38" s="24"/>
+      <c r="P38" s="24"/>
+      <c r="Q38" s="24"/>
+      <c r="R38" s="24"/>
+      <c r="S38" s="24"/>
+      <c r="T38" s="24"/>
+      <c r="U38" s="24"/>
+      <c r="V38" s="24"/>
+      <c r="W38" s="24"/>
+      <c r="X38" s="24"/>
+      <c r="Y38" s="25"/>
       <c r="Z38" s="1"/>
       <c r="AA38" s="1"/>
       <c r="AB38" s="1"/>
@@ -30959,23 +30965,23 @@
       <c r="F39" s="13"/>
       <c r="G39" s="13"/>
       <c r="H39" s="14"/>
-      <c r="I39" s="25"/>
-      <c r="J39" s="26"/>
+      <c r="I39" s="26"/>
+      <c r="J39" s="27"/>
       <c r="K39" s="14"/>
-      <c r="L39" s="25"/>
-      <c r="M39" s="25"/>
-      <c r="N39" s="26"/>
+      <c r="L39" s="26"/>
+      <c r="M39" s="26"/>
+      <c r="N39" s="27"/>
       <c r="O39" s="14"/>
-      <c r="P39" s="25"/>
-      <c r="Q39" s="25"/>
-      <c r="R39" s="25"/>
-      <c r="S39" s="25"/>
-      <c r="T39" s="25"/>
-      <c r="U39" s="25"/>
-      <c r="V39" s="25"/>
-      <c r="W39" s="25"/>
-      <c r="X39" s="25"/>
-      <c r="Y39" s="26"/>
+      <c r="P39" s="26"/>
+      <c r="Q39" s="26"/>
+      <c r="R39" s="26"/>
+      <c r="S39" s="26"/>
+      <c r="T39" s="26"/>
+      <c r="U39" s="26"/>
+      <c r="V39" s="26"/>
+      <c r="W39" s="26"/>
+      <c r="X39" s="26"/>
+      <c r="Y39" s="27"/>
       <c r="Z39" s="1"/>
       <c r="AA39" s="1"/>
       <c r="AB39" s="1"/>
@@ -31738,23 +31744,23 @@
       <c r="F40" s="11"/>
       <c r="G40" s="11"/>
       <c r="H40" s="12"/>
-      <c r="I40" s="23"/>
-      <c r="J40" s="24"/>
+      <c r="I40" s="24"/>
+      <c r="J40" s="25"/>
       <c r="K40" s="12"/>
-      <c r="L40" s="23"/>
-      <c r="M40" s="23"/>
-      <c r="N40" s="24"/>
+      <c r="L40" s="24"/>
+      <c r="M40" s="24"/>
+      <c r="N40" s="25"/>
       <c r="O40" s="12"/>
-      <c r="P40" s="23"/>
-      <c r="Q40" s="23"/>
-      <c r="R40" s="23"/>
-      <c r="S40" s="23"/>
-      <c r="T40" s="23"/>
-      <c r="U40" s="23"/>
-      <c r="V40" s="23"/>
-      <c r="W40" s="23"/>
-      <c r="X40" s="23"/>
-      <c r="Y40" s="24"/>
+      <c r="P40" s="24"/>
+      <c r="Q40" s="24"/>
+      <c r="R40" s="24"/>
+      <c r="S40" s="24"/>
+      <c r="T40" s="24"/>
+      <c r="U40" s="24"/>
+      <c r="V40" s="24"/>
+      <c r="W40" s="24"/>
+      <c r="X40" s="24"/>
+      <c r="Y40" s="25"/>
       <c r="Z40" s="1"/>
       <c r="AA40" s="1"/>
       <c r="AB40" s="1"/>
@@ -32515,23 +32521,23 @@
       <c r="F41" s="13"/>
       <c r="G41" s="13"/>
       <c r="H41" s="14"/>
-      <c r="I41" s="25"/>
-      <c r="J41" s="26"/>
+      <c r="I41" s="26"/>
+      <c r="J41" s="27"/>
       <c r="K41" s="14"/>
-      <c r="L41" s="25"/>
-      <c r="M41" s="25"/>
-      <c r="N41" s="26"/>
+      <c r="L41" s="26"/>
+      <c r="M41" s="26"/>
+      <c r="N41" s="27"/>
       <c r="O41" s="14"/>
-      <c r="P41" s="25"/>
-      <c r="Q41" s="25"/>
-      <c r="R41" s="25"/>
-      <c r="S41" s="25"/>
-      <c r="T41" s="25"/>
-      <c r="U41" s="25"/>
-      <c r="V41" s="25"/>
-      <c r="W41" s="25"/>
-      <c r="X41" s="25"/>
-      <c r="Y41" s="26"/>
+      <c r="P41" s="26"/>
+      <c r="Q41" s="26"/>
+      <c r="R41" s="26"/>
+      <c r="S41" s="26"/>
+      <c r="T41" s="26"/>
+      <c r="U41" s="26"/>
+      <c r="V41" s="26"/>
+      <c r="W41" s="26"/>
+      <c r="X41" s="26"/>
+      <c r="Y41" s="27"/>
       <c r="Z41" s="1"/>
       <c r="AA41" s="1"/>
       <c r="AB41" s="1"/>
@@ -33294,23 +33300,23 @@
       <c r="F42" s="11"/>
       <c r="G42" s="11"/>
       <c r="H42" s="12"/>
-      <c r="I42" s="23"/>
-      <c r="J42" s="24"/>
+      <c r="I42" s="24"/>
+      <c r="J42" s="25"/>
       <c r="K42" s="12"/>
-      <c r="L42" s="23"/>
-      <c r="M42" s="23"/>
-      <c r="N42" s="24"/>
+      <c r="L42" s="24"/>
+      <c r="M42" s="24"/>
+      <c r="N42" s="25"/>
       <c r="O42" s="12"/>
-      <c r="P42" s="23"/>
-      <c r="Q42" s="23"/>
-      <c r="R42" s="23"/>
-      <c r="S42" s="23"/>
-      <c r="T42" s="23"/>
-      <c r="U42" s="23"/>
-      <c r="V42" s="23"/>
-      <c r="W42" s="23"/>
-      <c r="X42" s="23"/>
-      <c r="Y42" s="24"/>
+      <c r="P42" s="24"/>
+      <c r="Q42" s="24"/>
+      <c r="R42" s="24"/>
+      <c r="S42" s="24"/>
+      <c r="T42" s="24"/>
+      <c r="U42" s="24"/>
+      <c r="V42" s="24"/>
+      <c r="W42" s="24"/>
+      <c r="X42" s="24"/>
+      <c r="Y42" s="25"/>
       <c r="Z42" s="1"/>
       <c r="AA42" s="1"/>
       <c r="AB42" s="1"/>
@@ -34071,23 +34077,23 @@
       <c r="F43" s="13"/>
       <c r="G43" s="13"/>
       <c r="H43" s="14"/>
-      <c r="I43" s="25"/>
-      <c r="J43" s="26"/>
+      <c r="I43" s="26"/>
+      <c r="J43" s="27"/>
       <c r="K43" s="14"/>
-      <c r="L43" s="25"/>
-      <c r="M43" s="25"/>
-      <c r="N43" s="26"/>
+      <c r="L43" s="26"/>
+      <c r="M43" s="26"/>
+      <c r="N43" s="27"/>
       <c r="O43" s="14"/>
-      <c r="P43" s="25"/>
-      <c r="Q43" s="25"/>
-      <c r="R43" s="25"/>
-      <c r="S43" s="25"/>
-      <c r="T43" s="25"/>
-      <c r="U43" s="25"/>
-      <c r="V43" s="25"/>
-      <c r="W43" s="25"/>
-      <c r="X43" s="25"/>
-      <c r="Y43" s="26"/>
+      <c r="P43" s="26"/>
+      <c r="Q43" s="26"/>
+      <c r="R43" s="26"/>
+      <c r="S43" s="26"/>
+      <c r="T43" s="26"/>
+      <c r="U43" s="26"/>
+      <c r="V43" s="26"/>
+      <c r="W43" s="26"/>
+      <c r="X43" s="26"/>
+      <c r="Y43" s="27"/>
       <c r="Z43" s="1"/>
       <c r="AA43" s="1"/>
       <c r="AB43" s="1"/>
@@ -34850,23 +34856,23 @@
       <c r="F44" s="11"/>
       <c r="G44" s="11"/>
       <c r="H44" s="12"/>
-      <c r="I44" s="23"/>
-      <c r="J44" s="24"/>
+      <c r="I44" s="24"/>
+      <c r="J44" s="25"/>
       <c r="K44" s="12"/>
-      <c r="L44" s="23"/>
-      <c r="M44" s="23"/>
-      <c r="N44" s="24"/>
+      <c r="L44" s="24"/>
+      <c r="M44" s="24"/>
+      <c r="N44" s="25"/>
       <c r="O44" s="12"/>
-      <c r="P44" s="23"/>
-      <c r="Q44" s="23"/>
-      <c r="R44" s="23"/>
-      <c r="S44" s="23"/>
-      <c r="T44" s="23"/>
-      <c r="U44" s="23"/>
-      <c r="V44" s="23"/>
-      <c r="W44" s="23"/>
-      <c r="X44" s="23"/>
-      <c r="Y44" s="24"/>
+      <c r="P44" s="24"/>
+      <c r="Q44" s="24"/>
+      <c r="R44" s="24"/>
+      <c r="S44" s="24"/>
+      <c r="T44" s="24"/>
+      <c r="U44" s="24"/>
+      <c r="V44" s="24"/>
+      <c r="W44" s="24"/>
+      <c r="X44" s="24"/>
+      <c r="Y44" s="25"/>
       <c r="Z44" s="1"/>
       <c r="AA44" s="1"/>
       <c r="AB44" s="1"/>
@@ -35627,23 +35633,23 @@
       <c r="F45" s="13"/>
       <c r="G45" s="13"/>
       <c r="H45" s="14"/>
-      <c r="I45" s="25"/>
-      <c r="J45" s="26"/>
+      <c r="I45" s="26"/>
+      <c r="J45" s="27"/>
       <c r="K45" s="14"/>
-      <c r="L45" s="25"/>
-      <c r="M45" s="25"/>
-      <c r="N45" s="26"/>
+      <c r="L45" s="26"/>
+      <c r="M45" s="26"/>
+      <c r="N45" s="27"/>
       <c r="O45" s="14"/>
-      <c r="P45" s="25"/>
-      <c r="Q45" s="25"/>
-      <c r="R45" s="25"/>
-      <c r="S45" s="25"/>
-      <c r="T45" s="25"/>
-      <c r="U45" s="25"/>
-      <c r="V45" s="25"/>
-      <c r="W45" s="25"/>
-      <c r="X45" s="25"/>
-      <c r="Y45" s="26"/>
+      <c r="P45" s="26"/>
+      <c r="Q45" s="26"/>
+      <c r="R45" s="26"/>
+      <c r="S45" s="26"/>
+      <c r="T45" s="26"/>
+      <c r="U45" s="26"/>
+      <c r="V45" s="26"/>
+      <c r="W45" s="26"/>
+      <c r="X45" s="26"/>
+      <c r="Y45" s="27"/>
       <c r="Z45" s="1"/>
       <c r="AA45" s="1"/>
       <c r="AB45" s="1"/>
@@ -36406,23 +36412,23 @@
       <c r="F46" s="11"/>
       <c r="G46" s="11"/>
       <c r="H46" s="12"/>
-      <c r="I46" s="23"/>
-      <c r="J46" s="24"/>
+      <c r="I46" s="24"/>
+      <c r="J46" s="25"/>
       <c r="K46" s="12"/>
-      <c r="L46" s="23"/>
-      <c r="M46" s="23"/>
-      <c r="N46" s="24"/>
+      <c r="L46" s="24"/>
+      <c r="M46" s="24"/>
+      <c r="N46" s="25"/>
       <c r="O46" s="12"/>
-      <c r="P46" s="23"/>
-      <c r="Q46" s="23"/>
-      <c r="R46" s="23"/>
-      <c r="S46" s="23"/>
-      <c r="T46" s="23"/>
-      <c r="U46" s="23"/>
-      <c r="V46" s="23"/>
-      <c r="W46" s="23"/>
-      <c r="X46" s="23"/>
-      <c r="Y46" s="24"/>
+      <c r="P46" s="24"/>
+      <c r="Q46" s="24"/>
+      <c r="R46" s="24"/>
+      <c r="S46" s="24"/>
+      <c r="T46" s="24"/>
+      <c r="U46" s="24"/>
+      <c r="V46" s="24"/>
+      <c r="W46" s="24"/>
+      <c r="X46" s="24"/>
+      <c r="Y46" s="25"/>
       <c r="Z46" s="1"/>
       <c r="AA46" s="1"/>
       <c r="AB46" s="1"/>
@@ -37183,23 +37189,23 @@
       <c r="F47" s="13"/>
       <c r="G47" s="13"/>
       <c r="H47" s="14"/>
-      <c r="I47" s="25"/>
-      <c r="J47" s="26"/>
+      <c r="I47" s="26"/>
+      <c r="J47" s="27"/>
       <c r="K47" s="14"/>
-      <c r="L47" s="25"/>
-      <c r="M47" s="25"/>
-      <c r="N47" s="26"/>
+      <c r="L47" s="26"/>
+      <c r="M47" s="26"/>
+      <c r="N47" s="27"/>
       <c r="O47" s="14"/>
-      <c r="P47" s="25"/>
-      <c r="Q47" s="25"/>
-      <c r="R47" s="25"/>
-      <c r="S47" s="25"/>
-      <c r="T47" s="25"/>
-      <c r="U47" s="25"/>
-      <c r="V47" s="25"/>
-      <c r="W47" s="25"/>
-      <c r="X47" s="25"/>
-      <c r="Y47" s="26"/>
+      <c r="P47" s="26"/>
+      <c r="Q47" s="26"/>
+      <c r="R47" s="26"/>
+      <c r="S47" s="26"/>
+      <c r="T47" s="26"/>
+      <c r="U47" s="26"/>
+      <c r="V47" s="26"/>
+      <c r="W47" s="26"/>
+      <c r="X47" s="26"/>
+      <c r="Y47" s="27"/>
       <c r="Z47" s="1"/>
       <c r="AA47" s="1"/>
       <c r="AB47" s="1"/>
@@ -37962,23 +37968,23 @@
       <c r="F48" s="11"/>
       <c r="G48" s="11"/>
       <c r="H48" s="12"/>
-      <c r="I48" s="23"/>
-      <c r="J48" s="24"/>
+      <c r="I48" s="24"/>
+      <c r="J48" s="25"/>
       <c r="K48" s="12"/>
-      <c r="L48" s="23"/>
-      <c r="M48" s="23"/>
-      <c r="N48" s="24"/>
+      <c r="L48" s="24"/>
+      <c r="M48" s="24"/>
+      <c r="N48" s="25"/>
       <c r="O48" s="12"/>
-      <c r="P48" s="23"/>
-      <c r="Q48" s="23"/>
-      <c r="R48" s="23"/>
-      <c r="S48" s="23"/>
-      <c r="T48" s="23"/>
-      <c r="U48" s="23"/>
-      <c r="V48" s="23"/>
-      <c r="W48" s="23"/>
-      <c r="X48" s="23"/>
-      <c r="Y48" s="24"/>
+      <c r="P48" s="24"/>
+      <c r="Q48" s="24"/>
+      <c r="R48" s="24"/>
+      <c r="S48" s="24"/>
+      <c r="T48" s="24"/>
+      <c r="U48" s="24"/>
+      <c r="V48" s="24"/>
+      <c r="W48" s="24"/>
+      <c r="X48" s="24"/>
+      <c r="Y48" s="25"/>
       <c r="Z48" s="1"/>
       <c r="AA48" s="1"/>
       <c r="AB48" s="1"/>
@@ -38739,23 +38745,23 @@
       <c r="F49" s="13"/>
       <c r="G49" s="13"/>
       <c r="H49" s="14"/>
-      <c r="I49" s="25"/>
-      <c r="J49" s="26"/>
+      <c r="I49" s="26"/>
+      <c r="J49" s="27"/>
       <c r="K49" s="14"/>
-      <c r="L49" s="25"/>
-      <c r="M49" s="25"/>
-      <c r="N49" s="26"/>
+      <c r="L49" s="26"/>
+      <c r="M49" s="26"/>
+      <c r="N49" s="27"/>
       <c r="O49" s="14"/>
-      <c r="P49" s="25"/>
-      <c r="Q49" s="25"/>
-      <c r="R49" s="25"/>
-      <c r="S49" s="25"/>
-      <c r="T49" s="25"/>
-      <c r="U49" s="25"/>
-      <c r="V49" s="25"/>
-      <c r="W49" s="25"/>
-      <c r="X49" s="25"/>
-      <c r="Y49" s="26"/>
+      <c r="P49" s="26"/>
+      <c r="Q49" s="26"/>
+      <c r="R49" s="26"/>
+      <c r="S49" s="26"/>
+      <c r="T49" s="26"/>
+      <c r="U49" s="26"/>
+      <c r="V49" s="26"/>
+      <c r="W49" s="26"/>
+      <c r="X49" s="26"/>
+      <c r="Y49" s="27"/>
       <c r="Z49" s="1"/>
       <c r="AA49" s="1"/>
       <c r="AB49" s="1"/>
@@ -39518,23 +39524,23 @@
       <c r="F50" s="11"/>
       <c r="G50" s="11"/>
       <c r="H50" s="12"/>
-      <c r="I50" s="23"/>
-      <c r="J50" s="24"/>
+      <c r="I50" s="24"/>
+      <c r="J50" s="25"/>
       <c r="K50" s="12"/>
-      <c r="L50" s="23"/>
-      <c r="M50" s="23"/>
-      <c r="N50" s="24"/>
+      <c r="L50" s="24"/>
+      <c r="M50" s="24"/>
+      <c r="N50" s="25"/>
       <c r="O50" s="12"/>
-      <c r="P50" s="23"/>
-      <c r="Q50" s="23"/>
-      <c r="R50" s="23"/>
-      <c r="S50" s="23"/>
-      <c r="T50" s="23"/>
-      <c r="U50" s="23"/>
-      <c r="V50" s="23"/>
-      <c r="W50" s="23"/>
-      <c r="X50" s="23"/>
-      <c r="Y50" s="24"/>
+      <c r="P50" s="24"/>
+      <c r="Q50" s="24"/>
+      <c r="R50" s="24"/>
+      <c r="S50" s="24"/>
+      <c r="T50" s="24"/>
+      <c r="U50" s="24"/>
+      <c r="V50" s="24"/>
+      <c r="W50" s="24"/>
+      <c r="X50" s="24"/>
+      <c r="Y50" s="25"/>
       <c r="Z50" s="1"/>
       <c r="AA50" s="1"/>
       <c r="AB50" s="1"/>
@@ -40295,23 +40301,23 @@
       <c r="F51" s="13"/>
       <c r="G51" s="13"/>
       <c r="H51" s="14"/>
-      <c r="I51" s="25"/>
-      <c r="J51" s="26"/>
+      <c r="I51" s="26"/>
+      <c r="J51" s="27"/>
       <c r="K51" s="14"/>
-      <c r="L51" s="25"/>
-      <c r="M51" s="25"/>
-      <c r="N51" s="26"/>
+      <c r="L51" s="26"/>
+      <c r="M51" s="26"/>
+      <c r="N51" s="27"/>
       <c r="O51" s="14"/>
-      <c r="P51" s="25"/>
-      <c r="Q51" s="25"/>
-      <c r="R51" s="25"/>
-      <c r="S51" s="25"/>
-      <c r="T51" s="25"/>
-      <c r="U51" s="25"/>
-      <c r="V51" s="25"/>
-      <c r="W51" s="25"/>
-      <c r="X51" s="25"/>
-      <c r="Y51" s="26"/>
+      <c r="P51" s="26"/>
+      <c r="Q51" s="26"/>
+      <c r="R51" s="26"/>
+      <c r="S51" s="26"/>
+      <c r="T51" s="26"/>
+      <c r="U51" s="26"/>
+      <c r="V51" s="26"/>
+      <c r="W51" s="26"/>
+      <c r="X51" s="26"/>
+      <c r="Y51" s="27"/>
       <c r="Z51" s="1"/>
       <c r="AA51" s="1"/>
       <c r="AB51" s="1"/>
@@ -41074,23 +41080,23 @@
       <c r="F52" s="11"/>
       <c r="G52" s="11"/>
       <c r="H52" s="12"/>
-      <c r="I52" s="23"/>
-      <c r="J52" s="24"/>
+      <c r="I52" s="24"/>
+      <c r="J52" s="25"/>
       <c r="K52" s="12"/>
-      <c r="L52" s="23"/>
-      <c r="M52" s="23"/>
-      <c r="N52" s="24"/>
+      <c r="L52" s="24"/>
+      <c r="M52" s="24"/>
+      <c r="N52" s="25"/>
       <c r="O52" s="12"/>
-      <c r="P52" s="23"/>
-      <c r="Q52" s="23"/>
-      <c r="R52" s="23"/>
-      <c r="S52" s="23"/>
-      <c r="T52" s="23"/>
-      <c r="U52" s="23"/>
-      <c r="V52" s="23"/>
-      <c r="W52" s="23"/>
-      <c r="X52" s="23"/>
-      <c r="Y52" s="24"/>
+      <c r="P52" s="24"/>
+      <c r="Q52" s="24"/>
+      <c r="R52" s="24"/>
+      <c r="S52" s="24"/>
+      <c r="T52" s="24"/>
+      <c r="U52" s="24"/>
+      <c r="V52" s="24"/>
+      <c r="W52" s="24"/>
+      <c r="X52" s="24"/>
+      <c r="Y52" s="25"/>
       <c r="Z52" s="1"/>
       <c r="AA52" s="1"/>
       <c r="AB52" s="1"/>
@@ -41851,23 +41857,23 @@
       <c r="F53" s="13"/>
       <c r="G53" s="13"/>
       <c r="H53" s="14"/>
-      <c r="I53" s="25"/>
-      <c r="J53" s="26"/>
+      <c r="I53" s="26"/>
+      <c r="J53" s="27"/>
       <c r="K53" s="14"/>
-      <c r="L53" s="25"/>
-      <c r="M53" s="25"/>
-      <c r="N53" s="26"/>
+      <c r="L53" s="26"/>
+      <c r="M53" s="26"/>
+      <c r="N53" s="27"/>
       <c r="O53" s="14"/>
-      <c r="P53" s="25"/>
-      <c r="Q53" s="25"/>
-      <c r="R53" s="25"/>
-      <c r="S53" s="25"/>
-      <c r="T53" s="25"/>
-      <c r="U53" s="25"/>
-      <c r="V53" s="25"/>
-      <c r="W53" s="25"/>
-      <c r="X53" s="25"/>
-      <c r="Y53" s="26"/>
+      <c r="P53" s="26"/>
+      <c r="Q53" s="26"/>
+      <c r="R53" s="26"/>
+      <c r="S53" s="26"/>
+      <c r="T53" s="26"/>
+      <c r="U53" s="26"/>
+      <c r="V53" s="26"/>
+      <c r="W53" s="26"/>
+      <c r="X53" s="26"/>
+      <c r="Y53" s="27"/>
       <c r="Z53" s="1"/>
       <c r="AA53" s="1"/>
       <c r="AB53" s="1"/>
@@ -42630,23 +42636,23 @@
       <c r="F54" s="11"/>
       <c r="G54" s="11"/>
       <c r="H54" s="12"/>
-      <c r="I54" s="23"/>
-      <c r="J54" s="24"/>
+      <c r="I54" s="24"/>
+      <c r="J54" s="25"/>
       <c r="K54" s="12"/>
-      <c r="L54" s="23"/>
-      <c r="M54" s="23"/>
-      <c r="N54" s="24"/>
+      <c r="L54" s="24"/>
+      <c r="M54" s="24"/>
+      <c r="N54" s="25"/>
       <c r="O54" s="12"/>
-      <c r="P54" s="23"/>
-      <c r="Q54" s="23"/>
-      <c r="R54" s="23"/>
-      <c r="S54" s="23"/>
-      <c r="T54" s="23"/>
-      <c r="U54" s="23"/>
-      <c r="V54" s="23"/>
-      <c r="W54" s="23"/>
-      <c r="X54" s="23"/>
-      <c r="Y54" s="24"/>
+      <c r="P54" s="24"/>
+      <c r="Q54" s="24"/>
+      <c r="R54" s="24"/>
+      <c r="S54" s="24"/>
+      <c r="T54" s="24"/>
+      <c r="U54" s="24"/>
+      <c r="V54" s="24"/>
+      <c r="W54" s="24"/>
+      <c r="X54" s="24"/>
+      <c r="Y54" s="25"/>
       <c r="Z54" s="1"/>
       <c r="AA54" s="1"/>
       <c r="AB54" s="1"/>
@@ -43407,23 +43413,23 @@
       <c r="F55" s="13"/>
       <c r="G55" s="13"/>
       <c r="H55" s="14"/>
-      <c r="I55" s="25"/>
-      <c r="J55" s="26"/>
+      <c r="I55" s="26"/>
+      <c r="J55" s="27"/>
       <c r="K55" s="14"/>
-      <c r="L55" s="25"/>
-      <c r="M55" s="25"/>
-      <c r="N55" s="26"/>
+      <c r="L55" s="26"/>
+      <c r="M55" s="26"/>
+      <c r="N55" s="27"/>
       <c r="O55" s="14"/>
-      <c r="P55" s="25"/>
-      <c r="Q55" s="25"/>
-      <c r="R55" s="25"/>
-      <c r="S55" s="25"/>
-      <c r="T55" s="25"/>
-      <c r="U55" s="25"/>
-      <c r="V55" s="25"/>
-      <c r="W55" s="25"/>
-      <c r="X55" s="25"/>
-      <c r="Y55" s="26"/>
+      <c r="P55" s="26"/>
+      <c r="Q55" s="26"/>
+      <c r="R55" s="26"/>
+      <c r="S55" s="26"/>
+      <c r="T55" s="26"/>
+      <c r="U55" s="26"/>
+      <c r="V55" s="26"/>
+      <c r="W55" s="26"/>
+      <c r="X55" s="26"/>
+      <c r="Y55" s="27"/>
       <c r="Z55" s="1"/>
       <c r="AA55" s="1"/>
       <c r="AB55" s="1"/>
@@ -44186,23 +44192,23 @@
       <c r="F56" s="11"/>
       <c r="G56" s="11"/>
       <c r="H56" s="12"/>
-      <c r="I56" s="23"/>
-      <c r="J56" s="24"/>
+      <c r="I56" s="24"/>
+      <c r="J56" s="25"/>
       <c r="K56" s="12"/>
-      <c r="L56" s="23"/>
-      <c r="M56" s="23"/>
-      <c r="N56" s="24"/>
+      <c r="L56" s="24"/>
+      <c r="M56" s="24"/>
+      <c r="N56" s="25"/>
       <c r="O56" s="12"/>
-      <c r="P56" s="23"/>
-      <c r="Q56" s="23"/>
-      <c r="R56" s="23"/>
-      <c r="S56" s="23"/>
-      <c r="T56" s="23"/>
-      <c r="U56" s="23"/>
-      <c r="V56" s="23"/>
-      <c r="W56" s="23"/>
-      <c r="X56" s="23"/>
-      <c r="Y56" s="24"/>
+      <c r="P56" s="24"/>
+      <c r="Q56" s="24"/>
+      <c r="R56" s="24"/>
+      <c r="S56" s="24"/>
+      <c r="T56" s="24"/>
+      <c r="U56" s="24"/>
+      <c r="V56" s="24"/>
+      <c r="W56" s="24"/>
+      <c r="X56" s="24"/>
+      <c r="Y56" s="25"/>
       <c r="Z56" s="1"/>
       <c r="AA56" s="1"/>
       <c r="AB56" s="1"/>
@@ -44963,23 +44969,23 @@
       <c r="F57" s="13"/>
       <c r="G57" s="13"/>
       <c r="H57" s="14"/>
-      <c r="I57" s="25"/>
-      <c r="J57" s="26"/>
+      <c r="I57" s="26"/>
+      <c r="J57" s="27"/>
       <c r="K57" s="14"/>
-      <c r="L57" s="25"/>
-      <c r="M57" s="25"/>
-      <c r="N57" s="26"/>
+      <c r="L57" s="26"/>
+      <c r="M57" s="26"/>
+      <c r="N57" s="27"/>
       <c r="O57" s="14"/>
-      <c r="P57" s="25"/>
-      <c r="Q57" s="25"/>
-      <c r="R57" s="25"/>
-      <c r="S57" s="25"/>
-      <c r="T57" s="25"/>
-      <c r="U57" s="25"/>
-      <c r="V57" s="25"/>
-      <c r="W57" s="25"/>
-      <c r="X57" s="25"/>
-      <c r="Y57" s="26"/>
+      <c r="P57" s="26"/>
+      <c r="Q57" s="26"/>
+      <c r="R57" s="26"/>
+      <c r="S57" s="26"/>
+      <c r="T57" s="26"/>
+      <c r="U57" s="26"/>
+      <c r="V57" s="26"/>
+      <c r="W57" s="26"/>
+      <c r="X57" s="26"/>
+      <c r="Y57" s="27"/>
       <c r="Z57" s="1"/>
       <c r="AA57" s="1"/>
       <c r="AB57" s="1"/>
@@ -45742,23 +45748,23 @@
       <c r="F58" s="11"/>
       <c r="G58" s="11"/>
       <c r="H58" s="12"/>
-      <c r="I58" s="23"/>
-      <c r="J58" s="24"/>
+      <c r="I58" s="24"/>
+      <c r="J58" s="25"/>
       <c r="K58" s="12"/>
-      <c r="L58" s="23"/>
-      <c r="M58" s="23"/>
-      <c r="N58" s="24"/>
+      <c r="L58" s="24"/>
+      <c r="M58" s="24"/>
+      <c r="N58" s="25"/>
       <c r="O58" s="12"/>
-      <c r="P58" s="23"/>
-      <c r="Q58" s="23"/>
-      <c r="R58" s="23"/>
-      <c r="S58" s="23"/>
-      <c r="T58" s="23"/>
-      <c r="U58" s="23"/>
-      <c r="V58" s="23"/>
-      <c r="W58" s="23"/>
-      <c r="X58" s="23"/>
-      <c r="Y58" s="24"/>
+      <c r="P58" s="24"/>
+      <c r="Q58" s="24"/>
+      <c r="R58" s="24"/>
+      <c r="S58" s="24"/>
+      <c r="T58" s="24"/>
+      <c r="U58" s="24"/>
+      <c r="V58" s="24"/>
+      <c r="W58" s="24"/>
+      <c r="X58" s="24"/>
+      <c r="Y58" s="25"/>
       <c r="Z58" s="1"/>
       <c r="AA58" s="1"/>
       <c r="AB58" s="1"/>
@@ -46519,23 +46525,23 @@
       <c r="F59" s="13"/>
       <c r="G59" s="13"/>
       <c r="H59" s="14"/>
-      <c r="I59" s="25"/>
-      <c r="J59" s="26"/>
+      <c r="I59" s="26"/>
+      <c r="J59" s="27"/>
       <c r="K59" s="14"/>
-      <c r="L59" s="25"/>
-      <c r="M59" s="25"/>
-      <c r="N59" s="26"/>
+      <c r="L59" s="26"/>
+      <c r="M59" s="26"/>
+      <c r="N59" s="27"/>
       <c r="O59" s="14"/>
-      <c r="P59" s="25"/>
-      <c r="Q59" s="25"/>
-      <c r="R59" s="25"/>
-      <c r="S59" s="25"/>
-      <c r="T59" s="25"/>
-      <c r="U59" s="25"/>
-      <c r="V59" s="25"/>
-      <c r="W59" s="25"/>
-      <c r="X59" s="25"/>
-      <c r="Y59" s="26"/>
+      <c r="P59" s="26"/>
+      <c r="Q59" s="26"/>
+      <c r="R59" s="26"/>
+      <c r="S59" s="26"/>
+      <c r="T59" s="26"/>
+      <c r="U59" s="26"/>
+      <c r="V59" s="26"/>
+      <c r="W59" s="26"/>
+      <c r="X59" s="26"/>
+      <c r="Y59" s="27"/>
       <c r="Z59" s="1"/>
       <c r="AA59" s="1"/>
       <c r="AB59" s="1"/>
@@ -48079,21 +48085,21 @@
       <c r="J61" s="16"/>
       <c r="K61" s="16"/>
       <c r="L61" s="16"/>
-      <c r="M61" s="27"/>
-      <c r="N61" s="28" t="s">
+      <c r="M61" s="28"/>
+      <c r="N61" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="O61" s="29"/>
-      <c r="P61" s="29"/>
-      <c r="Q61" s="29"/>
-      <c r="R61" s="29"/>
-      <c r="S61" s="29"/>
-      <c r="T61" s="29"/>
-      <c r="U61" s="29"/>
-      <c r="V61" s="29"/>
-      <c r="W61" s="29"/>
-      <c r="X61" s="29"/>
-      <c r="Y61" s="34"/>
+      <c r="O61" s="30"/>
+      <c r="P61" s="30"/>
+      <c r="Q61" s="30"/>
+      <c r="R61" s="30"/>
+      <c r="S61" s="30"/>
+      <c r="T61" s="30"/>
+      <c r="U61" s="30"/>
+      <c r="V61" s="30"/>
+      <c r="W61" s="30"/>
+      <c r="X61" s="30"/>
+      <c r="Y61" s="35"/>
       <c r="Z61" s="1"/>
       <c r="AA61" s="1"/>
       <c r="AB61" s="1"/>
@@ -48858,19 +48864,19 @@
       <c r="J62" s="18"/>
       <c r="K62" s="18"/>
       <c r="L62" s="18"/>
-      <c r="M62" s="30"/>
-      <c r="N62" s="31"/>
-      <c r="O62" s="32"/>
-      <c r="P62" s="32"/>
-      <c r="Q62" s="32"/>
-      <c r="R62" s="32"/>
-      <c r="S62" s="32"/>
-      <c r="T62" s="32"/>
-      <c r="U62" s="32"/>
-      <c r="V62" s="32"/>
-      <c r="W62" s="32"/>
-      <c r="X62" s="32"/>
-      <c r="Y62" s="35"/>
+      <c r="M62" s="31"/>
+      <c r="N62" s="32"/>
+      <c r="O62" s="33"/>
+      <c r="P62" s="33"/>
+      <c r="Q62" s="33"/>
+      <c r="R62" s="33"/>
+      <c r="S62" s="33"/>
+      <c r="T62" s="33"/>
+      <c r="U62" s="33"/>
+      <c r="V62" s="33"/>
+      <c r="W62" s="33"/>
+      <c r="X62" s="33"/>
+      <c r="Y62" s="36"/>
       <c r="Z62" s="1"/>
       <c r="AA62" s="1"/>
       <c r="AB62" s="1"/>
@@ -49624,30 +49630,30 @@
     </row>
     <row r="63" spans="1:775">
       <c r="A63" s="1"/>
-      <c r="B63" s="5"/>
-      <c r="C63" s="5"/>
-      <c r="D63" s="5"/>
-      <c r="E63" s="5"/>
-      <c r="F63" s="5"/>
-      <c r="G63" s="5"/>
-      <c r="H63" s="5"/>
-      <c r="I63" s="5"/>
-      <c r="J63" s="5"/>
-      <c r="K63" s="5"/>
-      <c r="L63" s="5"/>
-      <c r="M63" s="5"/>
-      <c r="N63" s="5"/>
-      <c r="O63" s="5"/>
-      <c r="P63" s="5"/>
-      <c r="Q63" s="5"/>
-      <c r="R63" s="5"/>
-      <c r="S63" s="5"/>
-      <c r="T63" s="5"/>
-      <c r="U63" s="5"/>
-      <c r="V63" s="5"/>
-      <c r="W63" s="5"/>
-      <c r="X63" s="5"/>
-      <c r="Y63" s="5"/>
+      <c r="B63" s="19"/>
+      <c r="C63" s="19"/>
+      <c r="D63" s="19"/>
+      <c r="E63" s="19"/>
+      <c r="F63" s="19"/>
+      <c r="G63" s="19"/>
+      <c r="H63" s="19"/>
+      <c r="I63" s="19"/>
+      <c r="J63" s="19"/>
+      <c r="K63" s="19"/>
+      <c r="L63" s="19"/>
+      <c r="M63" s="19"/>
+      <c r="N63" s="19"/>
+      <c r="O63" s="19"/>
+      <c r="P63" s="19"/>
+      <c r="Q63" s="19"/>
+      <c r="R63" s="19"/>
+      <c r="S63" s="19"/>
+      <c r="T63" s="19"/>
+      <c r="U63" s="19"/>
+      <c r="V63" s="19"/>
+      <c r="W63" s="19"/>
+      <c r="X63" s="19"/>
+      <c r="Y63" s="19"/>
       <c r="Z63" s="1"/>
       <c r="AA63" s="1"/>
       <c r="AB63" s="1"/>
@@ -50401,30 +50407,30 @@
     </row>
     <row r="64" spans="1:775">
       <c r="A64" s="1"/>
-      <c r="B64" s="5"/>
-      <c r="C64" s="5"/>
-      <c r="D64" s="5"/>
-      <c r="E64" s="5"/>
-      <c r="F64" s="5"/>
-      <c r="G64" s="5"/>
-      <c r="H64" s="5"/>
-      <c r="I64" s="5"/>
-      <c r="J64" s="5"/>
-      <c r="K64" s="5"/>
-      <c r="L64" s="5"/>
-      <c r="M64" s="5"/>
-      <c r="N64" s="5"/>
-      <c r="O64" s="5"/>
-      <c r="P64" s="5"/>
-      <c r="Q64" s="5"/>
-      <c r="R64" s="5"/>
-      <c r="S64" s="5"/>
-      <c r="T64" s="5"/>
-      <c r="U64" s="5"/>
-      <c r="V64" s="5"/>
-      <c r="W64" s="5"/>
-      <c r="X64" s="5"/>
-      <c r="Y64" s="5"/>
+      <c r="B64" s="19"/>
+      <c r="C64" s="19"/>
+      <c r="D64" s="19"/>
+      <c r="E64" s="19"/>
+      <c r="F64" s="19"/>
+      <c r="G64" s="19"/>
+      <c r="H64" s="19"/>
+      <c r="I64" s="19"/>
+      <c r="J64" s="19"/>
+      <c r="K64" s="19"/>
+      <c r="L64" s="19"/>
+      <c r="M64" s="19"/>
+      <c r="N64" s="19"/>
+      <c r="O64" s="19"/>
+      <c r="P64" s="19"/>
+      <c r="Q64" s="19"/>
+      <c r="R64" s="19"/>
+      <c r="S64" s="19"/>
+      <c r="T64" s="19"/>
+      <c r="U64" s="19"/>
+      <c r="V64" s="19"/>
+      <c r="W64" s="19"/>
+      <c r="X64" s="19"/>
+      <c r="Y64" s="19"/>
       <c r="Z64" s="1"/>
       <c r="AA64" s="1"/>
       <c r="AB64" s="1"/>
@@ -51178,30 +51184,30 @@
     </row>
     <row r="65" spans="1:775">
       <c r="A65" s="1"/>
-      <c r="B65" s="5"/>
-      <c r="C65" s="5"/>
-      <c r="D65" s="5"/>
-      <c r="E65" s="5"/>
-      <c r="F65" s="5"/>
-      <c r="G65" s="5"/>
-      <c r="H65" s="5"/>
-      <c r="I65" s="5"/>
-      <c r="J65" s="5"/>
-      <c r="K65" s="5"/>
-      <c r="L65" s="5"/>
-      <c r="M65" s="5"/>
-      <c r="N65" s="5"/>
-      <c r="O65" s="5"/>
-      <c r="P65" s="5"/>
-      <c r="Q65" s="5"/>
-      <c r="R65" s="5"/>
-      <c r="S65" s="5"/>
-      <c r="T65" s="5"/>
-      <c r="U65" s="5"/>
-      <c r="V65" s="5"/>
-      <c r="W65" s="5"/>
-      <c r="X65" s="5"/>
-      <c r="Y65" s="5"/>
+      <c r="B65" s="19"/>
+      <c r="C65" s="19"/>
+      <c r="D65" s="19"/>
+      <c r="E65" s="19"/>
+      <c r="F65" s="19"/>
+      <c r="G65" s="19"/>
+      <c r="H65" s="19"/>
+      <c r="I65" s="19"/>
+      <c r="J65" s="19"/>
+      <c r="K65" s="19"/>
+      <c r="L65" s="19"/>
+      <c r="M65" s="19"/>
+      <c r="N65" s="19"/>
+      <c r="O65" s="19"/>
+      <c r="P65" s="19"/>
+      <c r="Q65" s="19"/>
+      <c r="R65" s="19"/>
+      <c r="S65" s="19"/>
+      <c r="T65" s="19"/>
+      <c r="U65" s="19"/>
+      <c r="V65" s="19"/>
+      <c r="W65" s="19"/>
+      <c r="X65" s="19"/>
+      <c r="Y65" s="19"/>
       <c r="Z65" s="1"/>
       <c r="AA65" s="1"/>
       <c r="AB65" s="1"/>
@@ -51955,30 +51961,30 @@
     </row>
     <row r="66" spans="1:775">
       <c r="A66" s="1"/>
-      <c r="B66" s="5"/>
-      <c r="C66" s="5"/>
-      <c r="D66" s="5"/>
-      <c r="E66" s="5"/>
-      <c r="F66" s="5"/>
-      <c r="G66" s="5"/>
-      <c r="H66" s="5"/>
-      <c r="I66" s="5"/>
-      <c r="J66" s="5"/>
-      <c r="K66" s="5"/>
-      <c r="L66" s="5"/>
-      <c r="M66" s="5"/>
-      <c r="N66" s="5"/>
-      <c r="O66" s="5"/>
-      <c r="P66" s="5"/>
-      <c r="Q66" s="5"/>
-      <c r="R66" s="5"/>
-      <c r="S66" s="5"/>
-      <c r="T66" s="5"/>
-      <c r="U66" s="5"/>
-      <c r="V66" s="5"/>
-      <c r="W66" s="5"/>
-      <c r="X66" s="5"/>
-      <c r="Y66" s="5"/>
+      <c r="B66" s="19"/>
+      <c r="C66" s="19"/>
+      <c r="D66" s="19"/>
+      <c r="E66" s="19"/>
+      <c r="F66" s="19"/>
+      <c r="G66" s="19"/>
+      <c r="H66" s="19"/>
+      <c r="I66" s="19"/>
+      <c r="J66" s="19"/>
+      <c r="K66" s="19"/>
+      <c r="L66" s="19"/>
+      <c r="M66" s="19"/>
+      <c r="N66" s="19"/>
+      <c r="O66" s="19"/>
+      <c r="P66" s="19"/>
+      <c r="Q66" s="19"/>
+      <c r="R66" s="19"/>
+      <c r="S66" s="19"/>
+      <c r="T66" s="19"/>
+      <c r="U66" s="19"/>
+      <c r="V66" s="19"/>
+      <c r="W66" s="19"/>
+      <c r="X66" s="19"/>
+      <c r="Y66" s="19"/>
       <c r="Z66" s="1"/>
       <c r="AA66" s="1"/>
       <c r="AB66" s="1"/>
@@ -52732,30 +52738,30 @@
     </row>
     <row r="67" spans="1:775">
       <c r="A67" s="1"/>
-      <c r="B67" s="5"/>
-      <c r="C67" s="5"/>
-      <c r="D67" s="5"/>
-      <c r="E67" s="5"/>
-      <c r="F67" s="5"/>
-      <c r="G67" s="5"/>
-      <c r="H67" s="5"/>
-      <c r="I67" s="5"/>
-      <c r="J67" s="5"/>
-      <c r="K67" s="5"/>
-      <c r="L67" s="5"/>
-      <c r="M67" s="5"/>
-      <c r="N67" s="5"/>
-      <c r="O67" s="5"/>
-      <c r="P67" s="5"/>
-      <c r="Q67" s="5"/>
-      <c r="R67" s="5"/>
-      <c r="S67" s="5"/>
-      <c r="T67" s="5"/>
-      <c r="U67" s="5"/>
-      <c r="V67" s="5"/>
-      <c r="W67" s="5"/>
-      <c r="X67" s="5"/>
-      <c r="Y67" s="5"/>
+      <c r="B67" s="19"/>
+      <c r="C67" s="19"/>
+      <c r="D67" s="19"/>
+      <c r="E67" s="19"/>
+      <c r="F67" s="19"/>
+      <c r="G67" s="19"/>
+      <c r="H67" s="19"/>
+      <c r="I67" s="19"/>
+      <c r="J67" s="19"/>
+      <c r="K67" s="19"/>
+      <c r="L67" s="19"/>
+      <c r="M67" s="19"/>
+      <c r="N67" s="19"/>
+      <c r="O67" s="19"/>
+      <c r="P67" s="19"/>
+      <c r="Q67" s="19"/>
+      <c r="R67" s="19"/>
+      <c r="S67" s="19"/>
+      <c r="T67" s="19"/>
+      <c r="U67" s="19"/>
+      <c r="V67" s="19"/>
+      <c r="W67" s="19"/>
+      <c r="X67" s="19"/>
+      <c r="Y67" s="19"/>
       <c r="Z67" s="1"/>
       <c r="AA67" s="1"/>
       <c r="AB67" s="1"/>
@@ -53509,30 +53515,30 @@
     </row>
     <row r="68" spans="1:775">
       <c r="A68" s="1"/>
-      <c r="B68" s="5"/>
-      <c r="C68" s="5"/>
-      <c r="D68" s="5"/>
-      <c r="E68" s="5"/>
-      <c r="F68" s="5"/>
-      <c r="G68" s="5"/>
-      <c r="H68" s="5"/>
-      <c r="I68" s="5"/>
-      <c r="J68" s="5"/>
-      <c r="K68" s="5"/>
-      <c r="L68" s="5"/>
-      <c r="M68" s="5"/>
-      <c r="N68" s="5"/>
-      <c r="O68" s="5"/>
-      <c r="P68" s="5"/>
-      <c r="Q68" s="5"/>
-      <c r="R68" s="5"/>
-      <c r="S68" s="5"/>
-      <c r="T68" s="5"/>
-      <c r="U68" s="5"/>
-      <c r="V68" s="5"/>
-      <c r="W68" s="5"/>
-      <c r="X68" s="5"/>
-      <c r="Y68" s="5"/>
+      <c r="B68" s="19"/>
+      <c r="C68" s="19"/>
+      <c r="D68" s="19"/>
+      <c r="E68" s="19"/>
+      <c r="F68" s="19"/>
+      <c r="G68" s="19"/>
+      <c r="H68" s="19"/>
+      <c r="I68" s="19"/>
+      <c r="J68" s="19"/>
+      <c r="K68" s="19"/>
+      <c r="L68" s="19"/>
+      <c r="M68" s="19"/>
+      <c r="N68" s="19"/>
+      <c r="O68" s="19"/>
+      <c r="P68" s="19"/>
+      <c r="Q68" s="19"/>
+      <c r="R68" s="19"/>
+      <c r="S68" s="19"/>
+      <c r="T68" s="19"/>
+      <c r="U68" s="19"/>
+      <c r="V68" s="19"/>
+      <c r="W68" s="19"/>
+      <c r="X68" s="19"/>
+      <c r="Y68" s="19"/>
       <c r="Z68" s="1"/>
       <c r="AA68" s="1"/>
       <c r="AB68" s="1"/>
@@ -54286,30 +54292,30 @@
     </row>
     <row r="69" spans="1:775">
       <c r="A69" s="1"/>
-      <c r="B69" s="5"/>
-      <c r="C69" s="5"/>
-      <c r="D69" s="5"/>
-      <c r="E69" s="5"/>
-      <c r="F69" s="5"/>
-      <c r="G69" s="5"/>
-      <c r="H69" s="5"/>
-      <c r="I69" s="5"/>
-      <c r="J69" s="5"/>
-      <c r="K69" s="5"/>
-      <c r="L69" s="5"/>
-      <c r="M69" s="5"/>
-      <c r="N69" s="5"/>
-      <c r="O69" s="5"/>
-      <c r="P69" s="5"/>
-      <c r="Q69" s="5"/>
-      <c r="R69" s="5"/>
-      <c r="S69" s="5"/>
-      <c r="T69" s="5"/>
-      <c r="U69" s="5"/>
-      <c r="V69" s="5"/>
-      <c r="W69" s="5"/>
-      <c r="X69" s="5"/>
-      <c r="Y69" s="5"/>
+      <c r="B69" s="19"/>
+      <c r="C69" s="19"/>
+      <c r="D69" s="19"/>
+      <c r="E69" s="19"/>
+      <c r="F69" s="19"/>
+      <c r="G69" s="19"/>
+      <c r="H69" s="19"/>
+      <c r="I69" s="19"/>
+      <c r="J69" s="19"/>
+      <c r="K69" s="19"/>
+      <c r="L69" s="19"/>
+      <c r="M69" s="19"/>
+      <c r="N69" s="19"/>
+      <c r="O69" s="19"/>
+      <c r="P69" s="19"/>
+      <c r="Q69" s="19"/>
+      <c r="R69" s="19"/>
+      <c r="S69" s="19"/>
+      <c r="T69" s="19"/>
+      <c r="U69" s="19"/>
+      <c r="V69" s="19"/>
+      <c r="W69" s="19"/>
+      <c r="X69" s="19"/>
+      <c r="Y69" s="19"/>
       <c r="Z69" s="1"/>
       <c r="AA69" s="1"/>
       <c r="AB69" s="1"/>
@@ -55853,21 +55859,21 @@
       <c r="J71" s="16"/>
       <c r="K71" s="16"/>
       <c r="L71" s="16"/>
-      <c r="M71" s="27"/>
-      <c r="N71" s="28" t="s">
+      <c r="M71" s="28"/>
+      <c r="N71" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="O71" s="29"/>
-      <c r="P71" s="29"/>
-      <c r="Q71" s="29"/>
-      <c r="R71" s="29"/>
-      <c r="S71" s="29"/>
-      <c r="T71" s="29"/>
-      <c r="U71" s="29"/>
-      <c r="V71" s="29"/>
-      <c r="W71" s="29"/>
-      <c r="X71" s="29"/>
-      <c r="Y71" s="34"/>
+      <c r="O71" s="30"/>
+      <c r="P71" s="30"/>
+      <c r="Q71" s="30"/>
+      <c r="R71" s="30"/>
+      <c r="S71" s="30"/>
+      <c r="T71" s="30"/>
+      <c r="U71" s="30"/>
+      <c r="V71" s="30"/>
+      <c r="W71" s="30"/>
+      <c r="X71" s="30"/>
+      <c r="Y71" s="35"/>
       <c r="Z71" s="1"/>
       <c r="AA71" s="1"/>
       <c r="AB71" s="1"/>
@@ -56632,19 +56638,19 @@
       <c r="J72" s="18"/>
       <c r="K72" s="18"/>
       <c r="L72" s="18"/>
-      <c r="M72" s="30"/>
-      <c r="N72" s="31"/>
-      <c r="O72" s="32"/>
-      <c r="P72" s="32"/>
-      <c r="Q72" s="32"/>
-      <c r="R72" s="32"/>
-      <c r="S72" s="32"/>
-      <c r="T72" s="32"/>
-      <c r="U72" s="32"/>
-      <c r="V72" s="32"/>
-      <c r="W72" s="32"/>
-      <c r="X72" s="32"/>
-      <c r="Y72" s="35"/>
+      <c r="M72" s="31"/>
+      <c r="N72" s="32"/>
+      <c r="O72" s="33"/>
+      <c r="P72" s="33"/>
+      <c r="Q72" s="33"/>
+      <c r="R72" s="33"/>
+      <c r="S72" s="33"/>
+      <c r="T72" s="33"/>
+      <c r="U72" s="33"/>
+      <c r="V72" s="33"/>
+      <c r="W72" s="33"/>
+      <c r="X72" s="33"/>
+      <c r="Y72" s="36"/>
       <c r="Z72" s="1"/>
       <c r="AA72" s="1"/>
       <c r="AB72" s="1"/>
@@ -57398,30 +57404,30 @@
     </row>
     <row r="73" spans="1:775">
       <c r="A73" s="1"/>
-      <c r="B73" s="5"/>
-      <c r="C73" s="5"/>
-      <c r="D73" s="5"/>
-      <c r="E73" s="5"/>
-      <c r="F73" s="5"/>
-      <c r="G73" s="5"/>
-      <c r="H73" s="5"/>
-      <c r="I73" s="5"/>
-      <c r="J73" s="5"/>
-      <c r="K73" s="5"/>
-      <c r="L73" s="5"/>
-      <c r="M73" s="5"/>
-      <c r="N73" s="5"/>
-      <c r="O73" s="5"/>
-      <c r="P73" s="5"/>
-      <c r="Q73" s="5"/>
-      <c r="R73" s="5"/>
-      <c r="S73" s="5"/>
-      <c r="T73" s="5"/>
-      <c r="U73" s="5"/>
-      <c r="V73" s="5"/>
-      <c r="W73" s="5"/>
-      <c r="X73" s="5"/>
-      <c r="Y73" s="5"/>
+      <c r="B73" s="19"/>
+      <c r="C73" s="19"/>
+      <c r="D73" s="19"/>
+      <c r="E73" s="19"/>
+      <c r="F73" s="19"/>
+      <c r="G73" s="19"/>
+      <c r="H73" s="19"/>
+      <c r="I73" s="19"/>
+      <c r="J73" s="19"/>
+      <c r="K73" s="19"/>
+      <c r="L73" s="19"/>
+      <c r="M73" s="19"/>
+      <c r="N73" s="19"/>
+      <c r="O73" s="19"/>
+      <c r="P73" s="19"/>
+      <c r="Q73" s="19"/>
+      <c r="R73" s="19"/>
+      <c r="S73" s="19"/>
+      <c r="T73" s="19"/>
+      <c r="U73" s="19"/>
+      <c r="V73" s="19"/>
+      <c r="W73" s="19"/>
+      <c r="X73" s="19"/>
+      <c r="Y73" s="19"/>
       <c r="Z73" s="1"/>
       <c r="AA73" s="1"/>
       <c r="AB73" s="1"/>
@@ -58175,30 +58181,30 @@
     </row>
     <row r="74" spans="1:775">
       <c r="A74" s="1"/>
-      <c r="B74" s="5"/>
-      <c r="C74" s="5"/>
-      <c r="D74" s="5"/>
-      <c r="E74" s="5"/>
-      <c r="F74" s="5"/>
-      <c r="G74" s="5"/>
-      <c r="H74" s="5"/>
-      <c r="I74" s="5"/>
-      <c r="J74" s="5"/>
-      <c r="K74" s="5"/>
-      <c r="L74" s="5"/>
-      <c r="M74" s="5"/>
-      <c r="N74" s="5"/>
-      <c r="O74" s="5"/>
-      <c r="P74" s="5"/>
-      <c r="Q74" s="5"/>
-      <c r="R74" s="5"/>
-      <c r="S74" s="5"/>
-      <c r="T74" s="5"/>
-      <c r="U74" s="5"/>
-      <c r="V74" s="5"/>
-      <c r="W74" s="5"/>
-      <c r="X74" s="5"/>
-      <c r="Y74" s="5"/>
+      <c r="B74" s="19"/>
+      <c r="C74" s="19"/>
+      <c r="D74" s="19"/>
+      <c r="E74" s="19"/>
+      <c r="F74" s="19"/>
+      <c r="G74" s="19"/>
+      <c r="H74" s="19"/>
+      <c r="I74" s="19"/>
+      <c r="J74" s="19"/>
+      <c r="K74" s="19"/>
+      <c r="L74" s="19"/>
+      <c r="M74" s="19"/>
+      <c r="N74" s="19"/>
+      <c r="O74" s="19"/>
+      <c r="P74" s="19"/>
+      <c r="Q74" s="19"/>
+      <c r="R74" s="19"/>
+      <c r="S74" s="19"/>
+      <c r="T74" s="19"/>
+      <c r="U74" s="19"/>
+      <c r="V74" s="19"/>
+      <c r="W74" s="19"/>
+      <c r="X74" s="19"/>
+      <c r="Y74" s="19"/>
       <c r="Z74" s="1"/>
       <c r="AA74" s="1"/>
       <c r="AB74" s="1"/>
@@ -58952,30 +58958,30 @@
     </row>
     <row r="75" spans="1:775">
       <c r="A75" s="1"/>
-      <c r="B75" s="5"/>
-      <c r="C75" s="5"/>
-      <c r="D75" s="5"/>
-      <c r="E75" s="5"/>
-      <c r="F75" s="5"/>
-      <c r="G75" s="5"/>
-      <c r="H75" s="5"/>
-      <c r="I75" s="5"/>
-      <c r="J75" s="5"/>
-      <c r="K75" s="5"/>
-      <c r="L75" s="5"/>
-      <c r="M75" s="5"/>
-      <c r="N75" s="5"/>
-      <c r="O75" s="5"/>
-      <c r="P75" s="5"/>
-      <c r="Q75" s="5"/>
-      <c r="R75" s="5"/>
-      <c r="S75" s="5"/>
-      <c r="T75" s="5"/>
-      <c r="U75" s="5"/>
-      <c r="V75" s="5"/>
-      <c r="W75" s="5"/>
-      <c r="X75" s="5"/>
-      <c r="Y75" s="5"/>
+      <c r="B75" s="19"/>
+      <c r="C75" s="19"/>
+      <c r="D75" s="19"/>
+      <c r="E75" s="19"/>
+      <c r="F75" s="19"/>
+      <c r="G75" s="19"/>
+      <c r="H75" s="19"/>
+      <c r="I75" s="19"/>
+      <c r="J75" s="19"/>
+      <c r="K75" s="19"/>
+      <c r="L75" s="19"/>
+      <c r="M75" s="19"/>
+      <c r="N75" s="19"/>
+      <c r="O75" s="19"/>
+      <c r="P75" s="19"/>
+      <c r="Q75" s="19"/>
+      <c r="R75" s="19"/>
+      <c r="S75" s="19"/>
+      <c r="T75" s="19"/>
+      <c r="U75" s="19"/>
+      <c r="V75" s="19"/>
+      <c r="W75" s="19"/>
+      <c r="X75" s="19"/>
+      <c r="Y75" s="19"/>
       <c r="Z75" s="1"/>
       <c r="AA75" s="1"/>
       <c r="AB75" s="1"/>
@@ -59729,30 +59735,30 @@
     </row>
     <row r="76" spans="1:775">
       <c r="A76" s="1"/>
-      <c r="B76" s="5"/>
-      <c r="C76" s="5"/>
-      <c r="D76" s="5"/>
-      <c r="E76" s="5"/>
-      <c r="F76" s="5"/>
-      <c r="G76" s="5"/>
-      <c r="H76" s="5"/>
-      <c r="I76" s="5"/>
-      <c r="J76" s="5"/>
-      <c r="K76" s="5"/>
-      <c r="L76" s="5"/>
-      <c r="M76" s="5"/>
-      <c r="N76" s="5"/>
-      <c r="O76" s="5"/>
-      <c r="P76" s="5"/>
-      <c r="Q76" s="5"/>
-      <c r="R76" s="5"/>
-      <c r="S76" s="5"/>
-      <c r="T76" s="5"/>
-      <c r="U76" s="5"/>
-      <c r="V76" s="5"/>
-      <c r="W76" s="5"/>
-      <c r="X76" s="5"/>
-      <c r="Y76" s="5"/>
+      <c r="B76" s="19"/>
+      <c r="C76" s="19"/>
+      <c r="D76" s="19"/>
+      <c r="E76" s="19"/>
+      <c r="F76" s="19"/>
+      <c r="G76" s="19"/>
+      <c r="H76" s="19"/>
+      <c r="I76" s="19"/>
+      <c r="J76" s="19"/>
+      <c r="K76" s="19"/>
+      <c r="L76" s="19"/>
+      <c r="M76" s="19"/>
+      <c r="N76" s="19"/>
+      <c r="O76" s="19"/>
+      <c r="P76" s="19"/>
+      <c r="Q76" s="19"/>
+      <c r="R76" s="19"/>
+      <c r="S76" s="19"/>
+      <c r="T76" s="19"/>
+      <c r="U76" s="19"/>
+      <c r="V76" s="19"/>
+      <c r="W76" s="19"/>
+      <c r="X76" s="19"/>
+      <c r="Y76" s="19"/>
       <c r="Z76" s="1"/>
       <c r="AA76" s="1"/>
       <c r="AB76" s="1"/>
@@ -60506,30 +60512,30 @@
     </row>
     <row r="77" spans="1:775">
       <c r="A77" s="1"/>
-      <c r="B77" s="5"/>
-      <c r="C77" s="5"/>
-      <c r="D77" s="5"/>
-      <c r="E77" s="5"/>
-      <c r="F77" s="5"/>
-      <c r="G77" s="5"/>
-      <c r="H77" s="5"/>
-      <c r="I77" s="5"/>
-      <c r="J77" s="5"/>
-      <c r="K77" s="5"/>
-      <c r="L77" s="5"/>
-      <c r="M77" s="5"/>
-      <c r="N77" s="5"/>
-      <c r="O77" s="5"/>
-      <c r="P77" s="5"/>
-      <c r="Q77" s="5"/>
-      <c r="R77" s="5"/>
-      <c r="S77" s="5"/>
-      <c r="T77" s="5"/>
-      <c r="U77" s="5"/>
-      <c r="V77" s="5"/>
-      <c r="W77" s="5"/>
-      <c r="X77" s="5"/>
-      <c r="Y77" s="5"/>
+      <c r="B77" s="19"/>
+      <c r="C77" s="19"/>
+      <c r="D77" s="19"/>
+      <c r="E77" s="19"/>
+      <c r="F77" s="19"/>
+      <c r="G77" s="19"/>
+      <c r="H77" s="19"/>
+      <c r="I77" s="19"/>
+      <c r="J77" s="19"/>
+      <c r="K77" s="19"/>
+      <c r="L77" s="19"/>
+      <c r="M77" s="19"/>
+      <c r="N77" s="19"/>
+      <c r="O77" s="19"/>
+      <c r="P77" s="19"/>
+      <c r="Q77" s="19"/>
+      <c r="R77" s="19"/>
+      <c r="S77" s="19"/>
+      <c r="T77" s="19"/>
+      <c r="U77" s="19"/>
+      <c r="V77" s="19"/>
+      <c r="W77" s="19"/>
+      <c r="X77" s="19"/>
+      <c r="Y77" s="19"/>
       <c r="Z77" s="1"/>
       <c r="AA77" s="1"/>
       <c r="AB77" s="1"/>
@@ -61282,56 +61288,56 @@
       <c r="ACU77" s="1"/>
     </row>
     <row r="78" spans="2:25">
-      <c r="B78" s="5"/>
-      <c r="C78" s="5"/>
-      <c r="D78" s="5"/>
-      <c r="E78" s="5"/>
-      <c r="F78" s="5"/>
-      <c r="G78" s="5"/>
-      <c r="H78" s="5"/>
-      <c r="I78" s="5"/>
-      <c r="J78" s="5"/>
-      <c r="K78" s="5"/>
-      <c r="L78" s="5"/>
-      <c r="M78" s="5"/>
-      <c r="N78" s="5"/>
-      <c r="O78" s="5"/>
-      <c r="P78" s="5"/>
-      <c r="Q78" s="5"/>
-      <c r="R78" s="5"/>
-      <c r="S78" s="5"/>
-      <c r="T78" s="5"/>
-      <c r="U78" s="5"/>
-      <c r="V78" s="5"/>
-      <c r="W78" s="5"/>
-      <c r="X78" s="5"/>
-      <c r="Y78" s="5"/>
+      <c r="B78" s="19"/>
+      <c r="C78" s="19"/>
+      <c r="D78" s="19"/>
+      <c r="E78" s="19"/>
+      <c r="F78" s="19"/>
+      <c r="G78" s="19"/>
+      <c r="H78" s="19"/>
+      <c r="I78" s="19"/>
+      <c r="J78" s="19"/>
+      <c r="K78" s="19"/>
+      <c r="L78" s="19"/>
+      <c r="M78" s="19"/>
+      <c r="N78" s="19"/>
+      <c r="O78" s="19"/>
+      <c r="P78" s="19"/>
+      <c r="Q78" s="19"/>
+      <c r="R78" s="19"/>
+      <c r="S78" s="19"/>
+      <c r="T78" s="19"/>
+      <c r="U78" s="19"/>
+      <c r="V78" s="19"/>
+      <c r="W78" s="19"/>
+      <c r="X78" s="19"/>
+      <c r="Y78" s="19"/>
     </row>
     <row r="79" spans="2:25">
-      <c r="B79" s="5"/>
-      <c r="C79" s="5"/>
-      <c r="D79" s="5"/>
-      <c r="E79" s="5"/>
-      <c r="F79" s="5"/>
-      <c r="G79" s="5"/>
-      <c r="H79" s="5"/>
-      <c r="I79" s="5"/>
-      <c r="J79" s="5"/>
-      <c r="K79" s="5"/>
-      <c r="L79" s="5"/>
-      <c r="M79" s="5"/>
-      <c r="N79" s="5"/>
-      <c r="O79" s="5"/>
-      <c r="P79" s="5"/>
-      <c r="Q79" s="5"/>
-      <c r="R79" s="5"/>
-      <c r="S79" s="5"/>
-      <c r="T79" s="5"/>
-      <c r="U79" s="5"/>
-      <c r="V79" s="5"/>
-      <c r="W79" s="5"/>
-      <c r="X79" s="5"/>
-      <c r="Y79" s="5"/>
+      <c r="B79" s="19"/>
+      <c r="C79" s="19"/>
+      <c r="D79" s="19"/>
+      <c r="E79" s="19"/>
+      <c r="F79" s="19"/>
+      <c r="G79" s="19"/>
+      <c r="H79" s="19"/>
+      <c r="I79" s="19"/>
+      <c r="J79" s="19"/>
+      <c r="K79" s="19"/>
+      <c r="L79" s="19"/>
+      <c r="M79" s="19"/>
+      <c r="N79" s="19"/>
+      <c r="O79" s="19"/>
+      <c r="P79" s="19"/>
+      <c r="Q79" s="19"/>
+      <c r="R79" s="19"/>
+      <c r="S79" s="19"/>
+      <c r="T79" s="19"/>
+      <c r="U79" s="19"/>
+      <c r="V79" s="19"/>
+      <c r="W79" s="19"/>
+      <c r="X79" s="19"/>
+      <c r="Y79" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="126">

</xml_diff>

<commit_message>
[#7645] fix contact book 0 excel
</commit_message>
<xml_diff>
--- a/storage/app/excel/contact_book_0.xlsx
+++ b/storage/app/excel/contact_book_0.xlsx
@@ -144,10 +144,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -165,16 +165,30 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -188,8 +202,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -204,7 +219,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -212,7 +227,30 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -226,16 +264,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -248,42 +278,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -302,8 +301,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -366,25 +366,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -402,7 +414,103 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -414,67 +522,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -486,61 +534,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -674,11 +674,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -694,6 +700,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -722,28 +737,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -765,9 +763,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -776,13 +776,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -794,134 +794,134 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="15" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="18" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -980,7 +980,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1000,11 +1000,41 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1026,6 +1056,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1363,8 +1399,8 @@
   <sheetPr/>
   <dimension ref="A1:ACU79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="B73" sqref="B73:Y79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -7633,7 +7669,7 @@
       <c r="V9" s="21"/>
       <c r="W9" s="21"/>
       <c r="X9" s="21"/>
-      <c r="Y9" s="34"/>
+      <c r="Y9" s="44"/>
       <c r="Z9" s="1"/>
       <c r="AA9" s="1"/>
       <c r="AB9" s="1"/>
@@ -9962,21 +9998,21 @@
       <c r="H12" s="12"/>
       <c r="I12" s="24"/>
       <c r="J12" s="25"/>
-      <c r="K12" s="12"/>
-      <c r="L12" s="24"/>
-      <c r="M12" s="24"/>
-      <c r="N12" s="25"/>
-      <c r="O12" s="12"/>
-      <c r="P12" s="24"/>
-      <c r="Q12" s="24"/>
-      <c r="R12" s="24"/>
-      <c r="S12" s="24"/>
-      <c r="T12" s="24"/>
-      <c r="U12" s="24"/>
-      <c r="V12" s="24"/>
-      <c r="W12" s="24"/>
-      <c r="X12" s="24"/>
-      <c r="Y12" s="25"/>
+      <c r="K12" s="26"/>
+      <c r="L12" s="27"/>
+      <c r="M12" s="27"/>
+      <c r="N12" s="28"/>
+      <c r="O12" s="29"/>
+      <c r="P12" s="30"/>
+      <c r="Q12" s="30"/>
+      <c r="R12" s="30"/>
+      <c r="S12" s="30"/>
+      <c r="T12" s="30"/>
+      <c r="U12" s="30"/>
+      <c r="V12" s="30"/>
+      <c r="W12" s="30"/>
+      <c r="X12" s="30"/>
+      <c r="Y12" s="45"/>
       <c r="Z12" s="1"/>
       <c r="AA12" s="1"/>
       <c r="AB12" s="1"/>
@@ -10737,23 +10773,23 @@
       <c r="F13" s="13"/>
       <c r="G13" s="13"/>
       <c r="H13" s="14"/>
-      <c r="I13" s="26"/>
-      <c r="J13" s="27"/>
-      <c r="K13" s="14"/>
-      <c r="L13" s="26"/>
-      <c r="M13" s="26"/>
-      <c r="N13" s="27"/>
-      <c r="O13" s="14"/>
-      <c r="P13" s="26"/>
-      <c r="Q13" s="26"/>
-      <c r="R13" s="26"/>
-      <c r="S13" s="26"/>
-      <c r="T13" s="26"/>
-      <c r="U13" s="26"/>
-      <c r="V13" s="26"/>
-      <c r="W13" s="26"/>
-      <c r="X13" s="26"/>
-      <c r="Y13" s="27"/>
+      <c r="I13" s="31"/>
+      <c r="J13" s="32"/>
+      <c r="K13" s="33"/>
+      <c r="L13" s="34"/>
+      <c r="M13" s="34"/>
+      <c r="N13" s="35"/>
+      <c r="O13" s="36"/>
+      <c r="P13" s="37"/>
+      <c r="Q13" s="37"/>
+      <c r="R13" s="37"/>
+      <c r="S13" s="37"/>
+      <c r="T13" s="37"/>
+      <c r="U13" s="37"/>
+      <c r="V13" s="37"/>
+      <c r="W13" s="37"/>
+      <c r="X13" s="37"/>
+      <c r="Y13" s="46"/>
       <c r="Z13" s="1"/>
       <c r="AA13" s="1"/>
       <c r="AB13" s="1"/>
@@ -11518,21 +11554,21 @@
       <c r="H14" s="12"/>
       <c r="I14" s="24"/>
       <c r="J14" s="25"/>
-      <c r="K14" s="12"/>
-      <c r="L14" s="24"/>
-      <c r="M14" s="24"/>
-      <c r="N14" s="25"/>
-      <c r="O14" s="12"/>
-      <c r="P14" s="24"/>
-      <c r="Q14" s="24"/>
-      <c r="R14" s="24"/>
-      <c r="S14" s="24"/>
-      <c r="T14" s="24"/>
-      <c r="U14" s="24"/>
-      <c r="V14" s="24"/>
-      <c r="W14" s="24"/>
-      <c r="X14" s="24"/>
-      <c r="Y14" s="25"/>
+      <c r="K14" s="26"/>
+      <c r="L14" s="27"/>
+      <c r="M14" s="27"/>
+      <c r="N14" s="28"/>
+      <c r="O14" s="29"/>
+      <c r="P14" s="30"/>
+      <c r="Q14" s="30"/>
+      <c r="R14" s="30"/>
+      <c r="S14" s="30"/>
+      <c r="T14" s="30"/>
+      <c r="U14" s="30"/>
+      <c r="V14" s="30"/>
+      <c r="W14" s="30"/>
+      <c r="X14" s="30"/>
+      <c r="Y14" s="45"/>
       <c r="Z14" s="1"/>
       <c r="AA14" s="1"/>
       <c r="AB14" s="1"/>
@@ -12293,23 +12329,23 @@
       <c r="F15" s="13"/>
       <c r="G15" s="13"/>
       <c r="H15" s="14"/>
-      <c r="I15" s="26"/>
-      <c r="J15" s="27"/>
-      <c r="K15" s="14"/>
-      <c r="L15" s="26"/>
-      <c r="M15" s="26"/>
-      <c r="N15" s="27"/>
-      <c r="O15" s="14"/>
-      <c r="P15" s="26"/>
-      <c r="Q15" s="26"/>
-      <c r="R15" s="26"/>
-      <c r="S15" s="26"/>
-      <c r="T15" s="26"/>
-      <c r="U15" s="26"/>
-      <c r="V15" s="26"/>
-      <c r="W15" s="26"/>
-      <c r="X15" s="26"/>
-      <c r="Y15" s="27"/>
+      <c r="I15" s="31"/>
+      <c r="J15" s="32"/>
+      <c r="K15" s="33"/>
+      <c r="L15" s="34"/>
+      <c r="M15" s="34"/>
+      <c r="N15" s="35"/>
+      <c r="O15" s="36"/>
+      <c r="P15" s="37"/>
+      <c r="Q15" s="37"/>
+      <c r="R15" s="37"/>
+      <c r="S15" s="37"/>
+      <c r="T15" s="37"/>
+      <c r="U15" s="37"/>
+      <c r="V15" s="37"/>
+      <c r="W15" s="37"/>
+      <c r="X15" s="37"/>
+      <c r="Y15" s="46"/>
       <c r="Z15" s="1"/>
       <c r="AA15" s="1"/>
       <c r="AB15" s="1"/>
@@ -13074,21 +13110,21 @@
       <c r="H16" s="12"/>
       <c r="I16" s="24"/>
       <c r="J16" s="25"/>
-      <c r="K16" s="12"/>
-      <c r="L16" s="24"/>
-      <c r="M16" s="24"/>
-      <c r="N16" s="25"/>
-      <c r="O16" s="12"/>
-      <c r="P16" s="24"/>
-      <c r="Q16" s="24"/>
-      <c r="R16" s="24"/>
-      <c r="S16" s="24"/>
-      <c r="T16" s="24"/>
-      <c r="U16" s="24"/>
-      <c r="V16" s="24"/>
-      <c r="W16" s="24"/>
-      <c r="X16" s="24"/>
-      <c r="Y16" s="25"/>
+      <c r="K16" s="26"/>
+      <c r="L16" s="27"/>
+      <c r="M16" s="27"/>
+      <c r="N16" s="28"/>
+      <c r="O16" s="29"/>
+      <c r="P16" s="30"/>
+      <c r="Q16" s="30"/>
+      <c r="R16" s="30"/>
+      <c r="S16" s="30"/>
+      <c r="T16" s="30"/>
+      <c r="U16" s="30"/>
+      <c r="V16" s="30"/>
+      <c r="W16" s="30"/>
+      <c r="X16" s="30"/>
+      <c r="Y16" s="45"/>
       <c r="Z16" s="1"/>
       <c r="AA16" s="1"/>
       <c r="AB16" s="1"/>
@@ -13849,23 +13885,23 @@
       <c r="F17" s="13"/>
       <c r="G17" s="13"/>
       <c r="H17" s="14"/>
-      <c r="I17" s="26"/>
-      <c r="J17" s="27"/>
-      <c r="K17" s="14"/>
-      <c r="L17" s="26"/>
-      <c r="M17" s="26"/>
-      <c r="N17" s="27"/>
-      <c r="O17" s="14"/>
-      <c r="P17" s="26"/>
-      <c r="Q17" s="26"/>
-      <c r="R17" s="26"/>
-      <c r="S17" s="26"/>
-      <c r="T17" s="26"/>
-      <c r="U17" s="26"/>
-      <c r="V17" s="26"/>
-      <c r="W17" s="26"/>
-      <c r="X17" s="26"/>
-      <c r="Y17" s="27"/>
+      <c r="I17" s="31"/>
+      <c r="J17" s="32"/>
+      <c r="K17" s="33"/>
+      <c r="L17" s="34"/>
+      <c r="M17" s="34"/>
+      <c r="N17" s="35"/>
+      <c r="O17" s="36"/>
+      <c r="P17" s="37"/>
+      <c r="Q17" s="37"/>
+      <c r="R17" s="37"/>
+      <c r="S17" s="37"/>
+      <c r="T17" s="37"/>
+      <c r="U17" s="37"/>
+      <c r="V17" s="37"/>
+      <c r="W17" s="37"/>
+      <c r="X17" s="37"/>
+      <c r="Y17" s="46"/>
       <c r="Z17" s="1"/>
       <c r="AA17" s="1"/>
       <c r="AB17" s="1"/>
@@ -14630,21 +14666,21 @@
       <c r="H18" s="12"/>
       <c r="I18" s="24"/>
       <c r="J18" s="25"/>
-      <c r="K18" s="12"/>
-      <c r="L18" s="24"/>
-      <c r="M18" s="24"/>
-      <c r="N18" s="25"/>
-      <c r="O18" s="12"/>
-      <c r="P18" s="24"/>
-      <c r="Q18" s="24"/>
-      <c r="R18" s="24"/>
-      <c r="S18" s="24"/>
-      <c r="T18" s="24"/>
-      <c r="U18" s="24"/>
-      <c r="V18" s="24"/>
-      <c r="W18" s="24"/>
-      <c r="X18" s="24"/>
-      <c r="Y18" s="25"/>
+      <c r="K18" s="26"/>
+      <c r="L18" s="27"/>
+      <c r="M18" s="27"/>
+      <c r="N18" s="28"/>
+      <c r="O18" s="29"/>
+      <c r="P18" s="30"/>
+      <c r="Q18" s="30"/>
+      <c r="R18" s="30"/>
+      <c r="S18" s="30"/>
+      <c r="T18" s="30"/>
+      <c r="U18" s="30"/>
+      <c r="V18" s="30"/>
+      <c r="W18" s="30"/>
+      <c r="X18" s="30"/>
+      <c r="Y18" s="45"/>
       <c r="Z18" s="1"/>
       <c r="AA18" s="1"/>
       <c r="AB18" s="1"/>
@@ -15405,23 +15441,23 @@
       <c r="F19" s="13"/>
       <c r="G19" s="13"/>
       <c r="H19" s="14"/>
-      <c r="I19" s="26"/>
-      <c r="J19" s="27"/>
-      <c r="K19" s="14"/>
-      <c r="L19" s="26"/>
-      <c r="M19" s="26"/>
-      <c r="N19" s="27"/>
-      <c r="O19" s="14"/>
-      <c r="P19" s="26"/>
-      <c r="Q19" s="26"/>
-      <c r="R19" s="26"/>
-      <c r="S19" s="26"/>
-      <c r="T19" s="26"/>
-      <c r="U19" s="26"/>
-      <c r="V19" s="26"/>
-      <c r="W19" s="26"/>
-      <c r="X19" s="26"/>
-      <c r="Y19" s="27"/>
+      <c r="I19" s="31"/>
+      <c r="J19" s="32"/>
+      <c r="K19" s="33"/>
+      <c r="L19" s="34"/>
+      <c r="M19" s="34"/>
+      <c r="N19" s="35"/>
+      <c r="O19" s="36"/>
+      <c r="P19" s="37"/>
+      <c r="Q19" s="37"/>
+      <c r="R19" s="37"/>
+      <c r="S19" s="37"/>
+      <c r="T19" s="37"/>
+      <c r="U19" s="37"/>
+      <c r="V19" s="37"/>
+      <c r="W19" s="37"/>
+      <c r="X19" s="37"/>
+      <c r="Y19" s="46"/>
       <c r="Z19" s="1"/>
       <c r="AA19" s="1"/>
       <c r="AB19" s="1"/>
@@ -16186,21 +16222,21 @@
       <c r="H20" s="12"/>
       <c r="I20" s="24"/>
       <c r="J20" s="25"/>
-      <c r="K20" s="12"/>
-      <c r="L20" s="24"/>
-      <c r="M20" s="24"/>
-      <c r="N20" s="25"/>
-      <c r="O20" s="12"/>
-      <c r="P20" s="24"/>
-      <c r="Q20" s="24"/>
-      <c r="R20" s="24"/>
-      <c r="S20" s="24"/>
-      <c r="T20" s="24"/>
-      <c r="U20" s="24"/>
-      <c r="V20" s="24"/>
-      <c r="W20" s="24"/>
-      <c r="X20" s="24"/>
-      <c r="Y20" s="25"/>
+      <c r="K20" s="26"/>
+      <c r="L20" s="27"/>
+      <c r="M20" s="27"/>
+      <c r="N20" s="28"/>
+      <c r="O20" s="29"/>
+      <c r="P20" s="30"/>
+      <c r="Q20" s="30"/>
+      <c r="R20" s="30"/>
+      <c r="S20" s="30"/>
+      <c r="T20" s="30"/>
+      <c r="U20" s="30"/>
+      <c r="V20" s="30"/>
+      <c r="W20" s="30"/>
+      <c r="X20" s="30"/>
+      <c r="Y20" s="45"/>
       <c r="Z20" s="1"/>
       <c r="AA20" s="1"/>
       <c r="AB20" s="1"/>
@@ -16961,23 +16997,23 @@
       <c r="F21" s="13"/>
       <c r="G21" s="13"/>
       <c r="H21" s="14"/>
-      <c r="I21" s="26"/>
-      <c r="J21" s="27"/>
-      <c r="K21" s="14"/>
-      <c r="L21" s="26"/>
-      <c r="M21" s="26"/>
-      <c r="N21" s="27"/>
-      <c r="O21" s="14"/>
-      <c r="P21" s="26"/>
-      <c r="Q21" s="26"/>
-      <c r="R21" s="26"/>
-      <c r="S21" s="26"/>
-      <c r="T21" s="26"/>
-      <c r="U21" s="26"/>
-      <c r="V21" s="26"/>
-      <c r="W21" s="26"/>
-      <c r="X21" s="26"/>
-      <c r="Y21" s="27"/>
+      <c r="I21" s="31"/>
+      <c r="J21" s="32"/>
+      <c r="K21" s="33"/>
+      <c r="L21" s="34"/>
+      <c r="M21" s="34"/>
+      <c r="N21" s="35"/>
+      <c r="O21" s="36"/>
+      <c r="P21" s="37"/>
+      <c r="Q21" s="37"/>
+      <c r="R21" s="37"/>
+      <c r="S21" s="37"/>
+      <c r="T21" s="37"/>
+      <c r="U21" s="37"/>
+      <c r="V21" s="37"/>
+      <c r="W21" s="37"/>
+      <c r="X21" s="37"/>
+      <c r="Y21" s="46"/>
       <c r="Z21" s="1"/>
       <c r="AA21" s="1"/>
       <c r="AB21" s="1"/>
@@ -17742,21 +17778,21 @@
       <c r="H22" s="12"/>
       <c r="I22" s="24"/>
       <c r="J22" s="25"/>
-      <c r="K22" s="12"/>
-      <c r="L22" s="24"/>
-      <c r="M22" s="24"/>
-      <c r="N22" s="25"/>
-      <c r="O22" s="12"/>
-      <c r="P22" s="24"/>
-      <c r="Q22" s="24"/>
-      <c r="R22" s="24"/>
-      <c r="S22" s="24"/>
-      <c r="T22" s="24"/>
-      <c r="U22" s="24"/>
-      <c r="V22" s="24"/>
-      <c r="W22" s="24"/>
-      <c r="X22" s="24"/>
-      <c r="Y22" s="25"/>
+      <c r="K22" s="26"/>
+      <c r="L22" s="27"/>
+      <c r="M22" s="27"/>
+      <c r="N22" s="28"/>
+      <c r="O22" s="29"/>
+      <c r="P22" s="30"/>
+      <c r="Q22" s="30"/>
+      <c r="R22" s="30"/>
+      <c r="S22" s="30"/>
+      <c r="T22" s="30"/>
+      <c r="U22" s="30"/>
+      <c r="V22" s="30"/>
+      <c r="W22" s="30"/>
+      <c r="X22" s="30"/>
+      <c r="Y22" s="45"/>
       <c r="Z22" s="1"/>
       <c r="AA22" s="1"/>
       <c r="AB22" s="1"/>
@@ -18517,23 +18553,23 @@
       <c r="F23" s="13"/>
       <c r="G23" s="13"/>
       <c r="H23" s="14"/>
-      <c r="I23" s="26"/>
-      <c r="J23" s="27"/>
-      <c r="K23" s="14"/>
-      <c r="L23" s="26"/>
-      <c r="M23" s="26"/>
-      <c r="N23" s="27"/>
-      <c r="O23" s="14"/>
-      <c r="P23" s="26"/>
-      <c r="Q23" s="26"/>
-      <c r="R23" s="26"/>
-      <c r="S23" s="26"/>
-      <c r="T23" s="26"/>
-      <c r="U23" s="26"/>
-      <c r="V23" s="26"/>
-      <c r="W23" s="26"/>
-      <c r="X23" s="26"/>
-      <c r="Y23" s="27"/>
+      <c r="I23" s="31"/>
+      <c r="J23" s="32"/>
+      <c r="K23" s="33"/>
+      <c r="L23" s="34"/>
+      <c r="M23" s="34"/>
+      <c r="N23" s="35"/>
+      <c r="O23" s="36"/>
+      <c r="P23" s="37"/>
+      <c r="Q23" s="37"/>
+      <c r="R23" s="37"/>
+      <c r="S23" s="37"/>
+      <c r="T23" s="37"/>
+      <c r="U23" s="37"/>
+      <c r="V23" s="37"/>
+      <c r="W23" s="37"/>
+      <c r="X23" s="37"/>
+      <c r="Y23" s="46"/>
       <c r="Z23" s="1"/>
       <c r="AA23" s="1"/>
       <c r="AB23" s="1"/>
@@ -19298,21 +19334,21 @@
       <c r="H24" s="12"/>
       <c r="I24" s="24"/>
       <c r="J24" s="25"/>
-      <c r="K24" s="12"/>
-      <c r="L24" s="24"/>
-      <c r="M24" s="24"/>
-      <c r="N24" s="25"/>
-      <c r="O24" s="12"/>
-      <c r="P24" s="24"/>
-      <c r="Q24" s="24"/>
-      <c r="R24" s="24"/>
-      <c r="S24" s="24"/>
-      <c r="T24" s="24"/>
-      <c r="U24" s="24"/>
-      <c r="V24" s="24"/>
-      <c r="W24" s="24"/>
-      <c r="X24" s="24"/>
-      <c r="Y24" s="25"/>
+      <c r="K24" s="26"/>
+      <c r="L24" s="27"/>
+      <c r="M24" s="27"/>
+      <c r="N24" s="28"/>
+      <c r="O24" s="29"/>
+      <c r="P24" s="30"/>
+      <c r="Q24" s="30"/>
+      <c r="R24" s="30"/>
+      <c r="S24" s="30"/>
+      <c r="T24" s="30"/>
+      <c r="U24" s="30"/>
+      <c r="V24" s="30"/>
+      <c r="W24" s="30"/>
+      <c r="X24" s="30"/>
+      <c r="Y24" s="45"/>
       <c r="Z24" s="1"/>
       <c r="AA24" s="1"/>
       <c r="AB24" s="1"/>
@@ -20073,23 +20109,23 @@
       <c r="F25" s="13"/>
       <c r="G25" s="13"/>
       <c r="H25" s="14"/>
-      <c r="I25" s="26"/>
-      <c r="J25" s="27"/>
-      <c r="K25" s="14"/>
-      <c r="L25" s="26"/>
-      <c r="M25" s="26"/>
-      <c r="N25" s="27"/>
-      <c r="O25" s="14"/>
-      <c r="P25" s="26"/>
-      <c r="Q25" s="26"/>
-      <c r="R25" s="26"/>
-      <c r="S25" s="26"/>
-      <c r="T25" s="26"/>
-      <c r="U25" s="26"/>
-      <c r="V25" s="26"/>
-      <c r="W25" s="26"/>
-      <c r="X25" s="26"/>
-      <c r="Y25" s="27"/>
+      <c r="I25" s="31"/>
+      <c r="J25" s="32"/>
+      <c r="K25" s="33"/>
+      <c r="L25" s="34"/>
+      <c r="M25" s="34"/>
+      <c r="N25" s="35"/>
+      <c r="O25" s="36"/>
+      <c r="P25" s="37"/>
+      <c r="Q25" s="37"/>
+      <c r="R25" s="37"/>
+      <c r="S25" s="37"/>
+      <c r="T25" s="37"/>
+      <c r="U25" s="37"/>
+      <c r="V25" s="37"/>
+      <c r="W25" s="37"/>
+      <c r="X25" s="37"/>
+      <c r="Y25" s="46"/>
       <c r="Z25" s="1"/>
       <c r="AA25" s="1"/>
       <c r="AB25" s="1"/>
@@ -20854,21 +20890,21 @@
       <c r="H26" s="12"/>
       <c r="I26" s="24"/>
       <c r="J26" s="25"/>
-      <c r="K26" s="12"/>
-      <c r="L26" s="24"/>
-      <c r="M26" s="24"/>
-      <c r="N26" s="25"/>
-      <c r="O26" s="12"/>
-      <c r="P26" s="24"/>
-      <c r="Q26" s="24"/>
-      <c r="R26" s="24"/>
-      <c r="S26" s="24"/>
-      <c r="T26" s="24"/>
-      <c r="U26" s="24"/>
-      <c r="V26" s="24"/>
-      <c r="W26" s="24"/>
-      <c r="X26" s="24"/>
-      <c r="Y26" s="25"/>
+      <c r="K26" s="26"/>
+      <c r="L26" s="27"/>
+      <c r="M26" s="27"/>
+      <c r="N26" s="28"/>
+      <c r="O26" s="29"/>
+      <c r="P26" s="30"/>
+      <c r="Q26" s="30"/>
+      <c r="R26" s="30"/>
+      <c r="S26" s="30"/>
+      <c r="T26" s="30"/>
+      <c r="U26" s="30"/>
+      <c r="V26" s="30"/>
+      <c r="W26" s="30"/>
+      <c r="X26" s="30"/>
+      <c r="Y26" s="45"/>
       <c r="Z26" s="1"/>
       <c r="AA26" s="1"/>
       <c r="AB26" s="1"/>
@@ -21629,23 +21665,23 @@
       <c r="F27" s="13"/>
       <c r="G27" s="13"/>
       <c r="H27" s="14"/>
-      <c r="I27" s="26"/>
-      <c r="J27" s="27"/>
-      <c r="K27" s="14"/>
-      <c r="L27" s="26"/>
-      <c r="M27" s="26"/>
-      <c r="N27" s="27"/>
-      <c r="O27" s="14"/>
-      <c r="P27" s="26"/>
-      <c r="Q27" s="26"/>
-      <c r="R27" s="26"/>
-      <c r="S27" s="26"/>
-      <c r="T27" s="26"/>
-      <c r="U27" s="26"/>
-      <c r="V27" s="26"/>
-      <c r="W27" s="26"/>
-      <c r="X27" s="26"/>
-      <c r="Y27" s="27"/>
+      <c r="I27" s="31"/>
+      <c r="J27" s="32"/>
+      <c r="K27" s="33"/>
+      <c r="L27" s="34"/>
+      <c r="M27" s="34"/>
+      <c r="N27" s="35"/>
+      <c r="O27" s="36"/>
+      <c r="P27" s="37"/>
+      <c r="Q27" s="37"/>
+      <c r="R27" s="37"/>
+      <c r="S27" s="37"/>
+      <c r="T27" s="37"/>
+      <c r="U27" s="37"/>
+      <c r="V27" s="37"/>
+      <c r="W27" s="37"/>
+      <c r="X27" s="37"/>
+      <c r="Y27" s="46"/>
       <c r="Z27" s="1"/>
       <c r="AA27" s="1"/>
       <c r="AB27" s="1"/>
@@ -22410,21 +22446,21 @@
       <c r="H28" s="12"/>
       <c r="I28" s="24"/>
       <c r="J28" s="25"/>
-      <c r="K28" s="12"/>
-      <c r="L28" s="24"/>
-      <c r="M28" s="24"/>
-      <c r="N28" s="25"/>
-      <c r="O28" s="12"/>
-      <c r="P28" s="24"/>
-      <c r="Q28" s="24"/>
-      <c r="R28" s="24"/>
-      <c r="S28" s="24"/>
-      <c r="T28" s="24"/>
-      <c r="U28" s="24"/>
-      <c r="V28" s="24"/>
-      <c r="W28" s="24"/>
-      <c r="X28" s="24"/>
-      <c r="Y28" s="25"/>
+      <c r="K28" s="26"/>
+      <c r="L28" s="27"/>
+      <c r="M28" s="27"/>
+      <c r="N28" s="28"/>
+      <c r="O28" s="29"/>
+      <c r="P28" s="30"/>
+      <c r="Q28" s="30"/>
+      <c r="R28" s="30"/>
+      <c r="S28" s="30"/>
+      <c r="T28" s="30"/>
+      <c r="U28" s="30"/>
+      <c r="V28" s="30"/>
+      <c r="W28" s="30"/>
+      <c r="X28" s="30"/>
+      <c r="Y28" s="45"/>
       <c r="Z28" s="1"/>
       <c r="AA28" s="1"/>
       <c r="AB28" s="1"/>
@@ -23185,23 +23221,23 @@
       <c r="F29" s="13"/>
       <c r="G29" s="13"/>
       <c r="H29" s="14"/>
-      <c r="I29" s="26"/>
-      <c r="J29" s="27"/>
-      <c r="K29" s="14"/>
-      <c r="L29" s="26"/>
-      <c r="M29" s="26"/>
-      <c r="N29" s="27"/>
-      <c r="O29" s="14"/>
-      <c r="P29" s="26"/>
-      <c r="Q29" s="26"/>
-      <c r="R29" s="26"/>
-      <c r="S29" s="26"/>
-      <c r="T29" s="26"/>
-      <c r="U29" s="26"/>
-      <c r="V29" s="26"/>
-      <c r="W29" s="26"/>
-      <c r="X29" s="26"/>
-      <c r="Y29" s="27"/>
+      <c r="I29" s="31"/>
+      <c r="J29" s="32"/>
+      <c r="K29" s="33"/>
+      <c r="L29" s="34"/>
+      <c r="M29" s="34"/>
+      <c r="N29" s="35"/>
+      <c r="O29" s="36"/>
+      <c r="P29" s="37"/>
+      <c r="Q29" s="37"/>
+      <c r="R29" s="37"/>
+      <c r="S29" s="37"/>
+      <c r="T29" s="37"/>
+      <c r="U29" s="37"/>
+      <c r="V29" s="37"/>
+      <c r="W29" s="37"/>
+      <c r="X29" s="37"/>
+      <c r="Y29" s="46"/>
       <c r="Z29" s="1"/>
       <c r="AA29" s="1"/>
       <c r="AB29" s="1"/>
@@ -23966,21 +24002,21 @@
       <c r="H30" s="12"/>
       <c r="I30" s="24"/>
       <c r="J30" s="25"/>
-      <c r="K30" s="12"/>
-      <c r="L30" s="24"/>
-      <c r="M30" s="24"/>
-      <c r="N30" s="25"/>
-      <c r="O30" s="12"/>
-      <c r="P30" s="24"/>
-      <c r="Q30" s="24"/>
-      <c r="R30" s="24"/>
-      <c r="S30" s="24"/>
-      <c r="T30" s="24"/>
-      <c r="U30" s="24"/>
-      <c r="V30" s="24"/>
-      <c r="W30" s="24"/>
-      <c r="X30" s="24"/>
-      <c r="Y30" s="25"/>
+      <c r="K30" s="26"/>
+      <c r="L30" s="27"/>
+      <c r="M30" s="27"/>
+      <c r="N30" s="28"/>
+      <c r="O30" s="29"/>
+      <c r="P30" s="30"/>
+      <c r="Q30" s="30"/>
+      <c r="R30" s="30"/>
+      <c r="S30" s="30"/>
+      <c r="T30" s="30"/>
+      <c r="U30" s="30"/>
+      <c r="V30" s="30"/>
+      <c r="W30" s="30"/>
+      <c r="X30" s="30"/>
+      <c r="Y30" s="45"/>
       <c r="Z30" s="1"/>
       <c r="AA30" s="1"/>
       <c r="AB30" s="1"/>
@@ -24741,23 +24777,23 @@
       <c r="F31" s="13"/>
       <c r="G31" s="13"/>
       <c r="H31" s="14"/>
-      <c r="I31" s="26"/>
-      <c r="J31" s="27"/>
-      <c r="K31" s="14"/>
-      <c r="L31" s="26"/>
-      <c r="M31" s="26"/>
-      <c r="N31" s="27"/>
-      <c r="O31" s="14"/>
-      <c r="P31" s="26"/>
-      <c r="Q31" s="26"/>
-      <c r="R31" s="26"/>
-      <c r="S31" s="26"/>
-      <c r="T31" s="26"/>
-      <c r="U31" s="26"/>
-      <c r="V31" s="26"/>
-      <c r="W31" s="26"/>
-      <c r="X31" s="26"/>
-      <c r="Y31" s="27"/>
+      <c r="I31" s="31"/>
+      <c r="J31" s="32"/>
+      <c r="K31" s="33"/>
+      <c r="L31" s="34"/>
+      <c r="M31" s="34"/>
+      <c r="N31" s="35"/>
+      <c r="O31" s="36"/>
+      <c r="P31" s="37"/>
+      <c r="Q31" s="37"/>
+      <c r="R31" s="37"/>
+      <c r="S31" s="37"/>
+      <c r="T31" s="37"/>
+      <c r="U31" s="37"/>
+      <c r="V31" s="37"/>
+      <c r="W31" s="37"/>
+      <c r="X31" s="37"/>
+      <c r="Y31" s="46"/>
       <c r="Z31" s="1"/>
       <c r="AA31" s="1"/>
       <c r="AB31" s="1"/>
@@ -25522,21 +25558,21 @@
       <c r="H32" s="12"/>
       <c r="I32" s="24"/>
       <c r="J32" s="25"/>
-      <c r="K32" s="12"/>
-      <c r="L32" s="24"/>
-      <c r="M32" s="24"/>
-      <c r="N32" s="25"/>
-      <c r="O32" s="12"/>
-      <c r="P32" s="24"/>
-      <c r="Q32" s="24"/>
-      <c r="R32" s="24"/>
-      <c r="S32" s="24"/>
-      <c r="T32" s="24"/>
-      <c r="U32" s="24"/>
-      <c r="V32" s="24"/>
-      <c r="W32" s="24"/>
-      <c r="X32" s="24"/>
-      <c r="Y32" s="25"/>
+      <c r="K32" s="26"/>
+      <c r="L32" s="27"/>
+      <c r="M32" s="27"/>
+      <c r="N32" s="28"/>
+      <c r="O32" s="29"/>
+      <c r="P32" s="30"/>
+      <c r="Q32" s="30"/>
+      <c r="R32" s="30"/>
+      <c r="S32" s="30"/>
+      <c r="T32" s="30"/>
+      <c r="U32" s="30"/>
+      <c r="V32" s="30"/>
+      <c r="W32" s="30"/>
+      <c r="X32" s="30"/>
+      <c r="Y32" s="45"/>
       <c r="Z32" s="1"/>
       <c r="AA32" s="1"/>
       <c r="AB32" s="1"/>
@@ -26297,23 +26333,23 @@
       <c r="F33" s="13"/>
       <c r="G33" s="13"/>
       <c r="H33" s="14"/>
-      <c r="I33" s="26"/>
-      <c r="J33" s="27"/>
-      <c r="K33" s="14"/>
-      <c r="L33" s="26"/>
-      <c r="M33" s="26"/>
-      <c r="N33" s="27"/>
-      <c r="O33" s="14"/>
-      <c r="P33" s="26"/>
-      <c r="Q33" s="26"/>
-      <c r="R33" s="26"/>
-      <c r="S33" s="26"/>
-      <c r="T33" s="26"/>
-      <c r="U33" s="26"/>
-      <c r="V33" s="26"/>
-      <c r="W33" s="26"/>
-      <c r="X33" s="26"/>
-      <c r="Y33" s="27"/>
+      <c r="I33" s="31"/>
+      <c r="J33" s="32"/>
+      <c r="K33" s="33"/>
+      <c r="L33" s="34"/>
+      <c r="M33" s="34"/>
+      <c r="N33" s="35"/>
+      <c r="O33" s="36"/>
+      <c r="P33" s="37"/>
+      <c r="Q33" s="37"/>
+      <c r="R33" s="37"/>
+      <c r="S33" s="37"/>
+      <c r="T33" s="37"/>
+      <c r="U33" s="37"/>
+      <c r="V33" s="37"/>
+      <c r="W33" s="37"/>
+      <c r="X33" s="37"/>
+      <c r="Y33" s="46"/>
       <c r="Z33" s="1"/>
       <c r="AA33" s="1"/>
       <c r="AB33" s="1"/>
@@ -27078,21 +27114,21 @@
       <c r="H34" s="12"/>
       <c r="I34" s="24"/>
       <c r="J34" s="25"/>
-      <c r="K34" s="12"/>
-      <c r="L34" s="24"/>
-      <c r="M34" s="24"/>
-      <c r="N34" s="25"/>
-      <c r="O34" s="12"/>
-      <c r="P34" s="24"/>
-      <c r="Q34" s="24"/>
-      <c r="R34" s="24"/>
-      <c r="S34" s="24"/>
-      <c r="T34" s="24"/>
-      <c r="U34" s="24"/>
-      <c r="V34" s="24"/>
-      <c r="W34" s="24"/>
-      <c r="X34" s="24"/>
-      <c r="Y34" s="25"/>
+      <c r="K34" s="26"/>
+      <c r="L34" s="27"/>
+      <c r="M34" s="27"/>
+      <c r="N34" s="28"/>
+      <c r="O34" s="29"/>
+      <c r="P34" s="30"/>
+      <c r="Q34" s="30"/>
+      <c r="R34" s="30"/>
+      <c r="S34" s="30"/>
+      <c r="T34" s="30"/>
+      <c r="U34" s="30"/>
+      <c r="V34" s="30"/>
+      <c r="W34" s="30"/>
+      <c r="X34" s="30"/>
+      <c r="Y34" s="45"/>
       <c r="Z34" s="1"/>
       <c r="AA34" s="1"/>
       <c r="AB34" s="1"/>
@@ -27853,23 +27889,23 @@
       <c r="F35" s="13"/>
       <c r="G35" s="13"/>
       <c r="H35" s="14"/>
-      <c r="I35" s="26"/>
-      <c r="J35" s="27"/>
-      <c r="K35" s="14"/>
-      <c r="L35" s="26"/>
-      <c r="M35" s="26"/>
-      <c r="N35" s="27"/>
-      <c r="O35" s="14"/>
-      <c r="P35" s="26"/>
-      <c r="Q35" s="26"/>
-      <c r="R35" s="26"/>
-      <c r="S35" s="26"/>
-      <c r="T35" s="26"/>
-      <c r="U35" s="26"/>
-      <c r="V35" s="26"/>
-      <c r="W35" s="26"/>
-      <c r="X35" s="26"/>
-      <c r="Y35" s="27"/>
+      <c r="I35" s="31"/>
+      <c r="J35" s="32"/>
+      <c r="K35" s="33"/>
+      <c r="L35" s="34"/>
+      <c r="M35" s="34"/>
+      <c r="N35" s="35"/>
+      <c r="O35" s="36"/>
+      <c r="P35" s="37"/>
+      <c r="Q35" s="37"/>
+      <c r="R35" s="37"/>
+      <c r="S35" s="37"/>
+      <c r="T35" s="37"/>
+      <c r="U35" s="37"/>
+      <c r="V35" s="37"/>
+      <c r="W35" s="37"/>
+      <c r="X35" s="37"/>
+      <c r="Y35" s="46"/>
       <c r="Z35" s="1"/>
       <c r="AA35" s="1"/>
       <c r="AB35" s="1"/>
@@ -28634,21 +28670,21 @@
       <c r="H36" s="12"/>
       <c r="I36" s="24"/>
       <c r="J36" s="25"/>
-      <c r="K36" s="12"/>
-      <c r="L36" s="24"/>
-      <c r="M36" s="24"/>
-      <c r="N36" s="25"/>
-      <c r="O36" s="12"/>
-      <c r="P36" s="24"/>
-      <c r="Q36" s="24"/>
-      <c r="R36" s="24"/>
-      <c r="S36" s="24"/>
-      <c r="T36" s="24"/>
-      <c r="U36" s="24"/>
-      <c r="V36" s="24"/>
-      <c r="W36" s="24"/>
-      <c r="X36" s="24"/>
-      <c r="Y36" s="25"/>
+      <c r="K36" s="26"/>
+      <c r="L36" s="27"/>
+      <c r="M36" s="27"/>
+      <c r="N36" s="28"/>
+      <c r="O36" s="29"/>
+      <c r="P36" s="30"/>
+      <c r="Q36" s="30"/>
+      <c r="R36" s="30"/>
+      <c r="S36" s="30"/>
+      <c r="T36" s="30"/>
+      <c r="U36" s="30"/>
+      <c r="V36" s="30"/>
+      <c r="W36" s="30"/>
+      <c r="X36" s="30"/>
+      <c r="Y36" s="45"/>
       <c r="Z36" s="1"/>
       <c r="AA36" s="1"/>
       <c r="AB36" s="1"/>
@@ -29409,23 +29445,23 @@
       <c r="F37" s="13"/>
       <c r="G37" s="13"/>
       <c r="H37" s="14"/>
-      <c r="I37" s="26"/>
-      <c r="J37" s="27"/>
-      <c r="K37" s="14"/>
-      <c r="L37" s="26"/>
-      <c r="M37" s="26"/>
-      <c r="N37" s="27"/>
-      <c r="O37" s="14"/>
-      <c r="P37" s="26"/>
-      <c r="Q37" s="26"/>
-      <c r="R37" s="26"/>
-      <c r="S37" s="26"/>
-      <c r="T37" s="26"/>
-      <c r="U37" s="26"/>
-      <c r="V37" s="26"/>
-      <c r="W37" s="26"/>
-      <c r="X37" s="26"/>
-      <c r="Y37" s="27"/>
+      <c r="I37" s="31"/>
+      <c r="J37" s="32"/>
+      <c r="K37" s="33"/>
+      <c r="L37" s="34"/>
+      <c r="M37" s="34"/>
+      <c r="N37" s="35"/>
+      <c r="O37" s="36"/>
+      <c r="P37" s="37"/>
+      <c r="Q37" s="37"/>
+      <c r="R37" s="37"/>
+      <c r="S37" s="37"/>
+      <c r="T37" s="37"/>
+      <c r="U37" s="37"/>
+      <c r="V37" s="37"/>
+      <c r="W37" s="37"/>
+      <c r="X37" s="37"/>
+      <c r="Y37" s="46"/>
       <c r="Z37" s="1"/>
       <c r="AA37" s="1"/>
       <c r="AB37" s="1"/>
@@ -30190,21 +30226,21 @@
       <c r="H38" s="12"/>
       <c r="I38" s="24"/>
       <c r="J38" s="25"/>
-      <c r="K38" s="12"/>
-      <c r="L38" s="24"/>
-      <c r="M38" s="24"/>
-      <c r="N38" s="25"/>
-      <c r="O38" s="12"/>
-      <c r="P38" s="24"/>
-      <c r="Q38" s="24"/>
-      <c r="R38" s="24"/>
-      <c r="S38" s="24"/>
-      <c r="T38" s="24"/>
-      <c r="U38" s="24"/>
-      <c r="V38" s="24"/>
-      <c r="W38" s="24"/>
-      <c r="X38" s="24"/>
-      <c r="Y38" s="25"/>
+      <c r="K38" s="26"/>
+      <c r="L38" s="27"/>
+      <c r="M38" s="27"/>
+      <c r="N38" s="28"/>
+      <c r="O38" s="29"/>
+      <c r="P38" s="30"/>
+      <c r="Q38" s="30"/>
+      <c r="R38" s="30"/>
+      <c r="S38" s="30"/>
+      <c r="T38" s="30"/>
+      <c r="U38" s="30"/>
+      <c r="V38" s="30"/>
+      <c r="W38" s="30"/>
+      <c r="X38" s="30"/>
+      <c r="Y38" s="45"/>
       <c r="Z38" s="1"/>
       <c r="AA38" s="1"/>
       <c r="AB38" s="1"/>
@@ -30965,23 +31001,23 @@
       <c r="F39" s="13"/>
       <c r="G39" s="13"/>
       <c r="H39" s="14"/>
-      <c r="I39" s="26"/>
-      <c r="J39" s="27"/>
-      <c r="K39" s="14"/>
-      <c r="L39" s="26"/>
-      <c r="M39" s="26"/>
-      <c r="N39" s="27"/>
-      <c r="O39" s="14"/>
-      <c r="P39" s="26"/>
-      <c r="Q39" s="26"/>
-      <c r="R39" s="26"/>
-      <c r="S39" s="26"/>
-      <c r="T39" s="26"/>
-      <c r="U39" s="26"/>
-      <c r="V39" s="26"/>
-      <c r="W39" s="26"/>
-      <c r="X39" s="26"/>
-      <c r="Y39" s="27"/>
+      <c r="I39" s="31"/>
+      <c r="J39" s="32"/>
+      <c r="K39" s="33"/>
+      <c r="L39" s="34"/>
+      <c r="M39" s="34"/>
+      <c r="N39" s="35"/>
+      <c r="O39" s="36"/>
+      <c r="P39" s="37"/>
+      <c r="Q39" s="37"/>
+      <c r="R39" s="37"/>
+      <c r="S39" s="37"/>
+      <c r="T39" s="37"/>
+      <c r="U39" s="37"/>
+      <c r="V39" s="37"/>
+      <c r="W39" s="37"/>
+      <c r="X39" s="37"/>
+      <c r="Y39" s="46"/>
       <c r="Z39" s="1"/>
       <c r="AA39" s="1"/>
       <c r="AB39" s="1"/>
@@ -31746,21 +31782,21 @@
       <c r="H40" s="12"/>
       <c r="I40" s="24"/>
       <c r="J40" s="25"/>
-      <c r="K40" s="12"/>
-      <c r="L40" s="24"/>
-      <c r="M40" s="24"/>
-      <c r="N40" s="25"/>
-      <c r="O40" s="12"/>
-      <c r="P40" s="24"/>
-      <c r="Q40" s="24"/>
-      <c r="R40" s="24"/>
-      <c r="S40" s="24"/>
-      <c r="T40" s="24"/>
-      <c r="U40" s="24"/>
-      <c r="V40" s="24"/>
-      <c r="W40" s="24"/>
-      <c r="X40" s="24"/>
-      <c r="Y40" s="25"/>
+      <c r="K40" s="26"/>
+      <c r="L40" s="27"/>
+      <c r="M40" s="27"/>
+      <c r="N40" s="28"/>
+      <c r="O40" s="29"/>
+      <c r="P40" s="30"/>
+      <c r="Q40" s="30"/>
+      <c r="R40" s="30"/>
+      <c r="S40" s="30"/>
+      <c r="T40" s="30"/>
+      <c r="U40" s="30"/>
+      <c r="V40" s="30"/>
+      <c r="W40" s="30"/>
+      <c r="X40" s="30"/>
+      <c r="Y40" s="45"/>
       <c r="Z40" s="1"/>
       <c r="AA40" s="1"/>
       <c r="AB40" s="1"/>
@@ -32521,23 +32557,23 @@
       <c r="F41" s="13"/>
       <c r="G41" s="13"/>
       <c r="H41" s="14"/>
-      <c r="I41" s="26"/>
-      <c r="J41" s="27"/>
-      <c r="K41" s="14"/>
-      <c r="L41" s="26"/>
-      <c r="M41" s="26"/>
-      <c r="N41" s="27"/>
-      <c r="O41" s="14"/>
-      <c r="P41" s="26"/>
-      <c r="Q41" s="26"/>
-      <c r="R41" s="26"/>
-      <c r="S41" s="26"/>
-      <c r="T41" s="26"/>
-      <c r="U41" s="26"/>
-      <c r="V41" s="26"/>
-      <c r="W41" s="26"/>
-      <c r="X41" s="26"/>
-      <c r="Y41" s="27"/>
+      <c r="I41" s="31"/>
+      <c r="J41" s="32"/>
+      <c r="K41" s="33"/>
+      <c r="L41" s="34"/>
+      <c r="M41" s="34"/>
+      <c r="N41" s="35"/>
+      <c r="O41" s="36"/>
+      <c r="P41" s="37"/>
+      <c r="Q41" s="37"/>
+      <c r="R41" s="37"/>
+      <c r="S41" s="37"/>
+      <c r="T41" s="37"/>
+      <c r="U41" s="37"/>
+      <c r="V41" s="37"/>
+      <c r="W41" s="37"/>
+      <c r="X41" s="37"/>
+      <c r="Y41" s="46"/>
       <c r="Z41" s="1"/>
       <c r="AA41" s="1"/>
       <c r="AB41" s="1"/>
@@ -33302,21 +33338,21 @@
       <c r="H42" s="12"/>
       <c r="I42" s="24"/>
       <c r="J42" s="25"/>
-      <c r="K42" s="12"/>
-      <c r="L42" s="24"/>
-      <c r="M42" s="24"/>
-      <c r="N42" s="25"/>
-      <c r="O42" s="12"/>
-      <c r="P42" s="24"/>
-      <c r="Q42" s="24"/>
-      <c r="R42" s="24"/>
-      <c r="S42" s="24"/>
-      <c r="T42" s="24"/>
-      <c r="U42" s="24"/>
-      <c r="V42" s="24"/>
-      <c r="W42" s="24"/>
-      <c r="X42" s="24"/>
-      <c r="Y42" s="25"/>
+      <c r="K42" s="26"/>
+      <c r="L42" s="27"/>
+      <c r="M42" s="27"/>
+      <c r="N42" s="28"/>
+      <c r="O42" s="29"/>
+      <c r="P42" s="30"/>
+      <c r="Q42" s="30"/>
+      <c r="R42" s="30"/>
+      <c r="S42" s="30"/>
+      <c r="T42" s="30"/>
+      <c r="U42" s="30"/>
+      <c r="V42" s="30"/>
+      <c r="W42" s="30"/>
+      <c r="X42" s="30"/>
+      <c r="Y42" s="45"/>
       <c r="Z42" s="1"/>
       <c r="AA42" s="1"/>
       <c r="AB42" s="1"/>
@@ -34077,23 +34113,23 @@
       <c r="F43" s="13"/>
       <c r="G43" s="13"/>
       <c r="H43" s="14"/>
-      <c r="I43" s="26"/>
-      <c r="J43" s="27"/>
-      <c r="K43" s="14"/>
-      <c r="L43" s="26"/>
-      <c r="M43" s="26"/>
-      <c r="N43" s="27"/>
-      <c r="O43" s="14"/>
-      <c r="P43" s="26"/>
-      <c r="Q43" s="26"/>
-      <c r="R43" s="26"/>
-      <c r="S43" s="26"/>
-      <c r="T43" s="26"/>
-      <c r="U43" s="26"/>
-      <c r="V43" s="26"/>
-      <c r="W43" s="26"/>
-      <c r="X43" s="26"/>
-      <c r="Y43" s="27"/>
+      <c r="I43" s="31"/>
+      <c r="J43" s="32"/>
+      <c r="K43" s="33"/>
+      <c r="L43" s="34"/>
+      <c r="M43" s="34"/>
+      <c r="N43" s="35"/>
+      <c r="O43" s="36"/>
+      <c r="P43" s="37"/>
+      <c r="Q43" s="37"/>
+      <c r="R43" s="37"/>
+      <c r="S43" s="37"/>
+      <c r="T43" s="37"/>
+      <c r="U43" s="37"/>
+      <c r="V43" s="37"/>
+      <c r="W43" s="37"/>
+      <c r="X43" s="37"/>
+      <c r="Y43" s="46"/>
       <c r="Z43" s="1"/>
       <c r="AA43" s="1"/>
       <c r="AB43" s="1"/>
@@ -34858,21 +34894,21 @@
       <c r="H44" s="12"/>
       <c r="I44" s="24"/>
       <c r="J44" s="25"/>
-      <c r="K44" s="12"/>
-      <c r="L44" s="24"/>
-      <c r="M44" s="24"/>
-      <c r="N44" s="25"/>
-      <c r="O44" s="12"/>
-      <c r="P44" s="24"/>
-      <c r="Q44" s="24"/>
-      <c r="R44" s="24"/>
-      <c r="S44" s="24"/>
-      <c r="T44" s="24"/>
-      <c r="U44" s="24"/>
-      <c r="V44" s="24"/>
-      <c r="W44" s="24"/>
-      <c r="X44" s="24"/>
-      <c r="Y44" s="25"/>
+      <c r="K44" s="26"/>
+      <c r="L44" s="27"/>
+      <c r="M44" s="27"/>
+      <c r="N44" s="28"/>
+      <c r="O44" s="29"/>
+      <c r="P44" s="30"/>
+      <c r="Q44" s="30"/>
+      <c r="R44" s="30"/>
+      <c r="S44" s="30"/>
+      <c r="T44" s="30"/>
+      <c r="U44" s="30"/>
+      <c r="V44" s="30"/>
+      <c r="W44" s="30"/>
+      <c r="X44" s="30"/>
+      <c r="Y44" s="45"/>
       <c r="Z44" s="1"/>
       <c r="AA44" s="1"/>
       <c r="AB44" s="1"/>
@@ -35633,23 +35669,23 @@
       <c r="F45" s="13"/>
       <c r="G45" s="13"/>
       <c r="H45" s="14"/>
-      <c r="I45" s="26"/>
-      <c r="J45" s="27"/>
-      <c r="K45" s="14"/>
-      <c r="L45" s="26"/>
-      <c r="M45" s="26"/>
-      <c r="N45" s="27"/>
-      <c r="O45" s="14"/>
-      <c r="P45" s="26"/>
-      <c r="Q45" s="26"/>
-      <c r="R45" s="26"/>
-      <c r="S45" s="26"/>
-      <c r="T45" s="26"/>
-      <c r="U45" s="26"/>
-      <c r="V45" s="26"/>
-      <c r="W45" s="26"/>
-      <c r="X45" s="26"/>
-      <c r="Y45" s="27"/>
+      <c r="I45" s="31"/>
+      <c r="J45" s="32"/>
+      <c r="K45" s="33"/>
+      <c r="L45" s="34"/>
+      <c r="M45" s="34"/>
+      <c r="N45" s="35"/>
+      <c r="O45" s="36"/>
+      <c r="P45" s="37"/>
+      <c r="Q45" s="37"/>
+      <c r="R45" s="37"/>
+      <c r="S45" s="37"/>
+      <c r="T45" s="37"/>
+      <c r="U45" s="37"/>
+      <c r="V45" s="37"/>
+      <c r="W45" s="37"/>
+      <c r="X45" s="37"/>
+      <c r="Y45" s="46"/>
       <c r="Z45" s="1"/>
       <c r="AA45" s="1"/>
       <c r="AB45" s="1"/>
@@ -36414,21 +36450,21 @@
       <c r="H46" s="12"/>
       <c r="I46" s="24"/>
       <c r="J46" s="25"/>
-      <c r="K46" s="12"/>
-      <c r="L46" s="24"/>
-      <c r="M46" s="24"/>
-      <c r="N46" s="25"/>
-      <c r="O46" s="12"/>
-      <c r="P46" s="24"/>
-      <c r="Q46" s="24"/>
-      <c r="R46" s="24"/>
-      <c r="S46" s="24"/>
-      <c r="T46" s="24"/>
-      <c r="U46" s="24"/>
-      <c r="V46" s="24"/>
-      <c r="W46" s="24"/>
-      <c r="X46" s="24"/>
-      <c r="Y46" s="25"/>
+      <c r="K46" s="26"/>
+      <c r="L46" s="27"/>
+      <c r="M46" s="27"/>
+      <c r="N46" s="28"/>
+      <c r="O46" s="29"/>
+      <c r="P46" s="30"/>
+      <c r="Q46" s="30"/>
+      <c r="R46" s="30"/>
+      <c r="S46" s="30"/>
+      <c r="T46" s="30"/>
+      <c r="U46" s="30"/>
+      <c r="V46" s="30"/>
+      <c r="W46" s="30"/>
+      <c r="X46" s="30"/>
+      <c r="Y46" s="45"/>
       <c r="Z46" s="1"/>
       <c r="AA46" s="1"/>
       <c r="AB46" s="1"/>
@@ -37189,23 +37225,23 @@
       <c r="F47" s="13"/>
       <c r="G47" s="13"/>
       <c r="H47" s="14"/>
-      <c r="I47" s="26"/>
-      <c r="J47" s="27"/>
-      <c r="K47" s="14"/>
-      <c r="L47" s="26"/>
-      <c r="M47" s="26"/>
-      <c r="N47" s="27"/>
-      <c r="O47" s="14"/>
-      <c r="P47" s="26"/>
-      <c r="Q47" s="26"/>
-      <c r="R47" s="26"/>
-      <c r="S47" s="26"/>
-      <c r="T47" s="26"/>
-      <c r="U47" s="26"/>
-      <c r="V47" s="26"/>
-      <c r="W47" s="26"/>
-      <c r="X47" s="26"/>
-      <c r="Y47" s="27"/>
+      <c r="I47" s="31"/>
+      <c r="J47" s="32"/>
+      <c r="K47" s="33"/>
+      <c r="L47" s="34"/>
+      <c r="M47" s="34"/>
+      <c r="N47" s="35"/>
+      <c r="O47" s="36"/>
+      <c r="P47" s="37"/>
+      <c r="Q47" s="37"/>
+      <c r="R47" s="37"/>
+      <c r="S47" s="37"/>
+      <c r="T47" s="37"/>
+      <c r="U47" s="37"/>
+      <c r="V47" s="37"/>
+      <c r="W47" s="37"/>
+      <c r="X47" s="37"/>
+      <c r="Y47" s="46"/>
       <c r="Z47" s="1"/>
       <c r="AA47" s="1"/>
       <c r="AB47" s="1"/>
@@ -37970,21 +38006,21 @@
       <c r="H48" s="12"/>
       <c r="I48" s="24"/>
       <c r="J48" s="25"/>
-      <c r="K48" s="12"/>
-      <c r="L48" s="24"/>
-      <c r="M48" s="24"/>
-      <c r="N48" s="25"/>
-      <c r="O48" s="12"/>
-      <c r="P48" s="24"/>
-      <c r="Q48" s="24"/>
-      <c r="R48" s="24"/>
-      <c r="S48" s="24"/>
-      <c r="T48" s="24"/>
-      <c r="U48" s="24"/>
-      <c r="V48" s="24"/>
-      <c r="W48" s="24"/>
-      <c r="X48" s="24"/>
-      <c r="Y48" s="25"/>
+      <c r="K48" s="26"/>
+      <c r="L48" s="27"/>
+      <c r="M48" s="27"/>
+      <c r="N48" s="28"/>
+      <c r="O48" s="29"/>
+      <c r="P48" s="30"/>
+      <c r="Q48" s="30"/>
+      <c r="R48" s="30"/>
+      <c r="S48" s="30"/>
+      <c r="T48" s="30"/>
+      <c r="U48" s="30"/>
+      <c r="V48" s="30"/>
+      <c r="W48" s="30"/>
+      <c r="X48" s="30"/>
+      <c r="Y48" s="45"/>
       <c r="Z48" s="1"/>
       <c r="AA48" s="1"/>
       <c r="AB48" s="1"/>
@@ -38745,23 +38781,23 @@
       <c r="F49" s="13"/>
       <c r="G49" s="13"/>
       <c r="H49" s="14"/>
-      <c r="I49" s="26"/>
-      <c r="J49" s="27"/>
-      <c r="K49" s="14"/>
-      <c r="L49" s="26"/>
-      <c r="M49" s="26"/>
-      <c r="N49" s="27"/>
-      <c r="O49" s="14"/>
-      <c r="P49" s="26"/>
-      <c r="Q49" s="26"/>
-      <c r="R49" s="26"/>
-      <c r="S49" s="26"/>
-      <c r="T49" s="26"/>
-      <c r="U49" s="26"/>
-      <c r="V49" s="26"/>
-      <c r="W49" s="26"/>
-      <c r="X49" s="26"/>
-      <c r="Y49" s="27"/>
+      <c r="I49" s="31"/>
+      <c r="J49" s="32"/>
+      <c r="K49" s="33"/>
+      <c r="L49" s="34"/>
+      <c r="M49" s="34"/>
+      <c r="N49" s="35"/>
+      <c r="O49" s="36"/>
+      <c r="P49" s="37"/>
+      <c r="Q49" s="37"/>
+      <c r="R49" s="37"/>
+      <c r="S49" s="37"/>
+      <c r="T49" s="37"/>
+      <c r="U49" s="37"/>
+      <c r="V49" s="37"/>
+      <c r="W49" s="37"/>
+      <c r="X49" s="37"/>
+      <c r="Y49" s="46"/>
       <c r="Z49" s="1"/>
       <c r="AA49" s="1"/>
       <c r="AB49" s="1"/>
@@ -39526,21 +39562,21 @@
       <c r="H50" s="12"/>
       <c r="I50" s="24"/>
       <c r="J50" s="25"/>
-      <c r="K50" s="12"/>
-      <c r="L50" s="24"/>
-      <c r="M50" s="24"/>
-      <c r="N50" s="25"/>
-      <c r="O50" s="12"/>
-      <c r="P50" s="24"/>
-      <c r="Q50" s="24"/>
-      <c r="R50" s="24"/>
-      <c r="S50" s="24"/>
-      <c r="T50" s="24"/>
-      <c r="U50" s="24"/>
-      <c r="V50" s="24"/>
-      <c r="W50" s="24"/>
-      <c r="X50" s="24"/>
-      <c r="Y50" s="25"/>
+      <c r="K50" s="26"/>
+      <c r="L50" s="27"/>
+      <c r="M50" s="27"/>
+      <c r="N50" s="28"/>
+      <c r="O50" s="29"/>
+      <c r="P50" s="30"/>
+      <c r="Q50" s="30"/>
+      <c r="R50" s="30"/>
+      <c r="S50" s="30"/>
+      <c r="T50" s="30"/>
+      <c r="U50" s="30"/>
+      <c r="V50" s="30"/>
+      <c r="W50" s="30"/>
+      <c r="X50" s="30"/>
+      <c r="Y50" s="45"/>
       <c r="Z50" s="1"/>
       <c r="AA50" s="1"/>
       <c r="AB50" s="1"/>
@@ -40301,23 +40337,23 @@
       <c r="F51" s="13"/>
       <c r="G51" s="13"/>
       <c r="H51" s="14"/>
-      <c r="I51" s="26"/>
-      <c r="J51" s="27"/>
-      <c r="K51" s="14"/>
-      <c r="L51" s="26"/>
-      <c r="M51" s="26"/>
-      <c r="N51" s="27"/>
-      <c r="O51" s="14"/>
-      <c r="P51" s="26"/>
-      <c r="Q51" s="26"/>
-      <c r="R51" s="26"/>
-      <c r="S51" s="26"/>
-      <c r="T51" s="26"/>
-      <c r="U51" s="26"/>
-      <c r="V51" s="26"/>
-      <c r="W51" s="26"/>
-      <c r="X51" s="26"/>
-      <c r="Y51" s="27"/>
+      <c r="I51" s="31"/>
+      <c r="J51" s="32"/>
+      <c r="K51" s="33"/>
+      <c r="L51" s="34"/>
+      <c r="M51" s="34"/>
+      <c r="N51" s="35"/>
+      <c r="O51" s="36"/>
+      <c r="P51" s="37"/>
+      <c r="Q51" s="37"/>
+      <c r="R51" s="37"/>
+      <c r="S51" s="37"/>
+      <c r="T51" s="37"/>
+      <c r="U51" s="37"/>
+      <c r="V51" s="37"/>
+      <c r="W51" s="37"/>
+      <c r="X51" s="37"/>
+      <c r="Y51" s="46"/>
       <c r="Z51" s="1"/>
       <c r="AA51" s="1"/>
       <c r="AB51" s="1"/>
@@ -41082,21 +41118,21 @@
       <c r="H52" s="12"/>
       <c r="I52" s="24"/>
       <c r="J52" s="25"/>
-      <c r="K52" s="12"/>
-      <c r="L52" s="24"/>
-      <c r="M52" s="24"/>
-      <c r="N52" s="25"/>
-      <c r="O52" s="12"/>
-      <c r="P52" s="24"/>
-      <c r="Q52" s="24"/>
-      <c r="R52" s="24"/>
-      <c r="S52" s="24"/>
-      <c r="T52" s="24"/>
-      <c r="U52" s="24"/>
-      <c r="V52" s="24"/>
-      <c r="W52" s="24"/>
-      <c r="X52" s="24"/>
-      <c r="Y52" s="25"/>
+      <c r="K52" s="26"/>
+      <c r="L52" s="27"/>
+      <c r="M52" s="27"/>
+      <c r="N52" s="28"/>
+      <c r="O52" s="29"/>
+      <c r="P52" s="30"/>
+      <c r="Q52" s="30"/>
+      <c r="R52" s="30"/>
+      <c r="S52" s="30"/>
+      <c r="T52" s="30"/>
+      <c r="U52" s="30"/>
+      <c r="V52" s="30"/>
+      <c r="W52" s="30"/>
+      <c r="X52" s="30"/>
+      <c r="Y52" s="45"/>
       <c r="Z52" s="1"/>
       <c r="AA52" s="1"/>
       <c r="AB52" s="1"/>
@@ -41857,23 +41893,23 @@
       <c r="F53" s="13"/>
       <c r="G53" s="13"/>
       <c r="H53" s="14"/>
-      <c r="I53" s="26"/>
-      <c r="J53" s="27"/>
-      <c r="K53" s="14"/>
-      <c r="L53" s="26"/>
-      <c r="M53" s="26"/>
-      <c r="N53" s="27"/>
-      <c r="O53" s="14"/>
-      <c r="P53" s="26"/>
-      <c r="Q53" s="26"/>
-      <c r="R53" s="26"/>
-      <c r="S53" s="26"/>
-      <c r="T53" s="26"/>
-      <c r="U53" s="26"/>
-      <c r="V53" s="26"/>
-      <c r="W53" s="26"/>
-      <c r="X53" s="26"/>
-      <c r="Y53" s="27"/>
+      <c r="I53" s="31"/>
+      <c r="J53" s="32"/>
+      <c r="K53" s="33"/>
+      <c r="L53" s="34"/>
+      <c r="M53" s="34"/>
+      <c r="N53" s="35"/>
+      <c r="O53" s="36"/>
+      <c r="P53" s="37"/>
+      <c r="Q53" s="37"/>
+      <c r="R53" s="37"/>
+      <c r="S53" s="37"/>
+      <c r="T53" s="37"/>
+      <c r="U53" s="37"/>
+      <c r="V53" s="37"/>
+      <c r="W53" s="37"/>
+      <c r="X53" s="37"/>
+      <c r="Y53" s="46"/>
       <c r="Z53" s="1"/>
       <c r="AA53" s="1"/>
       <c r="AB53" s="1"/>
@@ -42638,21 +42674,21 @@
       <c r="H54" s="12"/>
       <c r="I54" s="24"/>
       <c r="J54" s="25"/>
-      <c r="K54" s="12"/>
-      <c r="L54" s="24"/>
-      <c r="M54" s="24"/>
-      <c r="N54" s="25"/>
-      <c r="O54" s="12"/>
-      <c r="P54" s="24"/>
-      <c r="Q54" s="24"/>
-      <c r="R54" s="24"/>
-      <c r="S54" s="24"/>
-      <c r="T54" s="24"/>
-      <c r="U54" s="24"/>
-      <c r="V54" s="24"/>
-      <c r="W54" s="24"/>
-      <c r="X54" s="24"/>
-      <c r="Y54" s="25"/>
+      <c r="K54" s="26"/>
+      <c r="L54" s="27"/>
+      <c r="M54" s="27"/>
+      <c r="N54" s="28"/>
+      <c r="O54" s="29"/>
+      <c r="P54" s="30"/>
+      <c r="Q54" s="30"/>
+      <c r="R54" s="30"/>
+      <c r="S54" s="30"/>
+      <c r="T54" s="30"/>
+      <c r="U54" s="30"/>
+      <c r="V54" s="30"/>
+      <c r="W54" s="30"/>
+      <c r="X54" s="30"/>
+      <c r="Y54" s="45"/>
       <c r="Z54" s="1"/>
       <c r="AA54" s="1"/>
       <c r="AB54" s="1"/>
@@ -43413,23 +43449,23 @@
       <c r="F55" s="13"/>
       <c r="G55" s="13"/>
       <c r="H55" s="14"/>
-      <c r="I55" s="26"/>
-      <c r="J55" s="27"/>
-      <c r="K55" s="14"/>
-      <c r="L55" s="26"/>
-      <c r="M55" s="26"/>
-      <c r="N55" s="27"/>
-      <c r="O55" s="14"/>
-      <c r="P55" s="26"/>
-      <c r="Q55" s="26"/>
-      <c r="R55" s="26"/>
-      <c r="S55" s="26"/>
-      <c r="T55" s="26"/>
-      <c r="U55" s="26"/>
-      <c r="V55" s="26"/>
-      <c r="W55" s="26"/>
-      <c r="X55" s="26"/>
-      <c r="Y55" s="27"/>
+      <c r="I55" s="31"/>
+      <c r="J55" s="32"/>
+      <c r="K55" s="33"/>
+      <c r="L55" s="34"/>
+      <c r="M55" s="34"/>
+      <c r="N55" s="35"/>
+      <c r="O55" s="36"/>
+      <c r="P55" s="37"/>
+      <c r="Q55" s="37"/>
+      <c r="R55" s="37"/>
+      <c r="S55" s="37"/>
+      <c r="T55" s="37"/>
+      <c r="U55" s="37"/>
+      <c r="V55" s="37"/>
+      <c r="W55" s="37"/>
+      <c r="X55" s="37"/>
+      <c r="Y55" s="46"/>
       <c r="Z55" s="1"/>
       <c r="AA55" s="1"/>
       <c r="AB55" s="1"/>
@@ -44194,21 +44230,21 @@
       <c r="H56" s="12"/>
       <c r="I56" s="24"/>
       <c r="J56" s="25"/>
-      <c r="K56" s="12"/>
-      <c r="L56" s="24"/>
-      <c r="M56" s="24"/>
-      <c r="N56" s="25"/>
-      <c r="O56" s="12"/>
-      <c r="P56" s="24"/>
-      <c r="Q56" s="24"/>
-      <c r="R56" s="24"/>
-      <c r="S56" s="24"/>
-      <c r="T56" s="24"/>
-      <c r="U56" s="24"/>
-      <c r="V56" s="24"/>
-      <c r="W56" s="24"/>
-      <c r="X56" s="24"/>
-      <c r="Y56" s="25"/>
+      <c r="K56" s="26"/>
+      <c r="L56" s="27"/>
+      <c r="M56" s="27"/>
+      <c r="N56" s="28"/>
+      <c r="O56" s="29"/>
+      <c r="P56" s="30"/>
+      <c r="Q56" s="30"/>
+      <c r="R56" s="30"/>
+      <c r="S56" s="30"/>
+      <c r="T56" s="30"/>
+      <c r="U56" s="30"/>
+      <c r="V56" s="30"/>
+      <c r="W56" s="30"/>
+      <c r="X56" s="30"/>
+      <c r="Y56" s="45"/>
       <c r="Z56" s="1"/>
       <c r="AA56" s="1"/>
       <c r="AB56" s="1"/>
@@ -44969,23 +45005,23 @@
       <c r="F57" s="13"/>
       <c r="G57" s="13"/>
       <c r="H57" s="14"/>
-      <c r="I57" s="26"/>
-      <c r="J57" s="27"/>
-      <c r="K57" s="14"/>
-      <c r="L57" s="26"/>
-      <c r="M57" s="26"/>
-      <c r="N57" s="27"/>
-      <c r="O57" s="14"/>
-      <c r="P57" s="26"/>
-      <c r="Q57" s="26"/>
-      <c r="R57" s="26"/>
-      <c r="S57" s="26"/>
-      <c r="T57" s="26"/>
-      <c r="U57" s="26"/>
-      <c r="V57" s="26"/>
-      <c r="W57" s="26"/>
-      <c r="X57" s="26"/>
-      <c r="Y57" s="27"/>
+      <c r="I57" s="31"/>
+      <c r="J57" s="32"/>
+      <c r="K57" s="33"/>
+      <c r="L57" s="34"/>
+      <c r="M57" s="34"/>
+      <c r="N57" s="35"/>
+      <c r="O57" s="36"/>
+      <c r="P57" s="37"/>
+      <c r="Q57" s="37"/>
+      <c r="R57" s="37"/>
+      <c r="S57" s="37"/>
+      <c r="T57" s="37"/>
+      <c r="U57" s="37"/>
+      <c r="V57" s="37"/>
+      <c r="W57" s="37"/>
+      <c r="X57" s="37"/>
+      <c r="Y57" s="46"/>
       <c r="Z57" s="1"/>
       <c r="AA57" s="1"/>
       <c r="AB57" s="1"/>
@@ -45750,21 +45786,21 @@
       <c r="H58" s="12"/>
       <c r="I58" s="24"/>
       <c r="J58" s="25"/>
-      <c r="K58" s="12"/>
-      <c r="L58" s="24"/>
-      <c r="M58" s="24"/>
-      <c r="N58" s="25"/>
-      <c r="O58" s="12"/>
-      <c r="P58" s="24"/>
-      <c r="Q58" s="24"/>
-      <c r="R58" s="24"/>
-      <c r="S58" s="24"/>
-      <c r="T58" s="24"/>
-      <c r="U58" s="24"/>
-      <c r="V58" s="24"/>
-      <c r="W58" s="24"/>
-      <c r="X58" s="24"/>
-      <c r="Y58" s="25"/>
+      <c r="K58" s="26"/>
+      <c r="L58" s="27"/>
+      <c r="M58" s="27"/>
+      <c r="N58" s="28"/>
+      <c r="O58" s="29"/>
+      <c r="P58" s="30"/>
+      <c r="Q58" s="30"/>
+      <c r="R58" s="30"/>
+      <c r="S58" s="30"/>
+      <c r="T58" s="30"/>
+      <c r="U58" s="30"/>
+      <c r="V58" s="30"/>
+      <c r="W58" s="30"/>
+      <c r="X58" s="30"/>
+      <c r="Y58" s="45"/>
       <c r="Z58" s="1"/>
       <c r="AA58" s="1"/>
       <c r="AB58" s="1"/>
@@ -46525,23 +46561,23 @@
       <c r="F59" s="13"/>
       <c r="G59" s="13"/>
       <c r="H59" s="14"/>
-      <c r="I59" s="26"/>
-      <c r="J59" s="27"/>
-      <c r="K59" s="14"/>
-      <c r="L59" s="26"/>
-      <c r="M59" s="26"/>
-      <c r="N59" s="27"/>
-      <c r="O59" s="14"/>
-      <c r="P59" s="26"/>
-      <c r="Q59" s="26"/>
-      <c r="R59" s="26"/>
-      <c r="S59" s="26"/>
-      <c r="T59" s="26"/>
-      <c r="U59" s="26"/>
-      <c r="V59" s="26"/>
-      <c r="W59" s="26"/>
-      <c r="X59" s="26"/>
-      <c r="Y59" s="27"/>
+      <c r="I59" s="31"/>
+      <c r="J59" s="32"/>
+      <c r="K59" s="33"/>
+      <c r="L59" s="34"/>
+      <c r="M59" s="34"/>
+      <c r="N59" s="35"/>
+      <c r="O59" s="36"/>
+      <c r="P59" s="37"/>
+      <c r="Q59" s="37"/>
+      <c r="R59" s="37"/>
+      <c r="S59" s="37"/>
+      <c r="T59" s="37"/>
+      <c r="U59" s="37"/>
+      <c r="V59" s="37"/>
+      <c r="W59" s="37"/>
+      <c r="X59" s="37"/>
+      <c r="Y59" s="46"/>
       <c r="Z59" s="1"/>
       <c r="AA59" s="1"/>
       <c r="AB59" s="1"/>
@@ -48085,21 +48121,21 @@
       <c r="J61" s="16"/>
       <c r="K61" s="16"/>
       <c r="L61" s="16"/>
-      <c r="M61" s="28"/>
-      <c r="N61" s="29" t="s">
+      <c r="M61" s="38"/>
+      <c r="N61" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="O61" s="30"/>
-      <c r="P61" s="30"/>
-      <c r="Q61" s="30"/>
-      <c r="R61" s="30"/>
-      <c r="S61" s="30"/>
-      <c r="T61" s="30"/>
-      <c r="U61" s="30"/>
-      <c r="V61" s="30"/>
-      <c r="W61" s="30"/>
-      <c r="X61" s="30"/>
-      <c r="Y61" s="35"/>
+      <c r="O61" s="40"/>
+      <c r="P61" s="40"/>
+      <c r="Q61" s="40"/>
+      <c r="R61" s="40"/>
+      <c r="S61" s="40"/>
+      <c r="T61" s="40"/>
+      <c r="U61" s="40"/>
+      <c r="V61" s="40"/>
+      <c r="W61" s="40"/>
+      <c r="X61" s="40"/>
+      <c r="Y61" s="47"/>
       <c r="Z61" s="1"/>
       <c r="AA61" s="1"/>
       <c r="AB61" s="1"/>
@@ -48864,19 +48900,19 @@
       <c r="J62" s="18"/>
       <c r="K62" s="18"/>
       <c r="L62" s="18"/>
-      <c r="M62" s="31"/>
-      <c r="N62" s="32"/>
-      <c r="O62" s="33"/>
-      <c r="P62" s="33"/>
-      <c r="Q62" s="33"/>
-      <c r="R62" s="33"/>
-      <c r="S62" s="33"/>
-      <c r="T62" s="33"/>
-      <c r="U62" s="33"/>
-      <c r="V62" s="33"/>
-      <c r="W62" s="33"/>
-      <c r="X62" s="33"/>
-      <c r="Y62" s="36"/>
+      <c r="M62" s="41"/>
+      <c r="N62" s="42"/>
+      <c r="O62" s="43"/>
+      <c r="P62" s="43"/>
+      <c r="Q62" s="43"/>
+      <c r="R62" s="43"/>
+      <c r="S62" s="43"/>
+      <c r="T62" s="43"/>
+      <c r="U62" s="43"/>
+      <c r="V62" s="43"/>
+      <c r="W62" s="43"/>
+      <c r="X62" s="43"/>
+      <c r="Y62" s="48"/>
       <c r="Z62" s="1"/>
       <c r="AA62" s="1"/>
       <c r="AB62" s="1"/>
@@ -55859,21 +55895,21 @@
       <c r="J71" s="16"/>
       <c r="K71" s="16"/>
       <c r="L71" s="16"/>
-      <c r="M71" s="28"/>
-      <c r="N71" s="29" t="s">
+      <c r="M71" s="38"/>
+      <c r="N71" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="O71" s="30"/>
-      <c r="P71" s="30"/>
-      <c r="Q71" s="30"/>
-      <c r="R71" s="30"/>
-      <c r="S71" s="30"/>
-      <c r="T71" s="30"/>
-      <c r="U71" s="30"/>
-      <c r="V71" s="30"/>
-      <c r="W71" s="30"/>
-      <c r="X71" s="30"/>
-      <c r="Y71" s="35"/>
+      <c r="O71" s="40"/>
+      <c r="P71" s="40"/>
+      <c r="Q71" s="40"/>
+      <c r="R71" s="40"/>
+      <c r="S71" s="40"/>
+      <c r="T71" s="40"/>
+      <c r="U71" s="40"/>
+      <c r="V71" s="40"/>
+      <c r="W71" s="40"/>
+      <c r="X71" s="40"/>
+      <c r="Y71" s="47"/>
       <c r="Z71" s="1"/>
       <c r="AA71" s="1"/>
       <c r="AB71" s="1"/>
@@ -56638,19 +56674,19 @@
       <c r="J72" s="18"/>
       <c r="K72" s="18"/>
       <c r="L72" s="18"/>
-      <c r="M72" s="31"/>
-      <c r="N72" s="32"/>
-      <c r="O72" s="33"/>
-      <c r="P72" s="33"/>
-      <c r="Q72" s="33"/>
-      <c r="R72" s="33"/>
-      <c r="S72" s="33"/>
-      <c r="T72" s="33"/>
-      <c r="U72" s="33"/>
-      <c r="V72" s="33"/>
-      <c r="W72" s="33"/>
-      <c r="X72" s="33"/>
-      <c r="Y72" s="36"/>
+      <c r="M72" s="41"/>
+      <c r="N72" s="42"/>
+      <c r="O72" s="43"/>
+      <c r="P72" s="43"/>
+      <c r="Q72" s="43"/>
+      <c r="R72" s="43"/>
+      <c r="S72" s="43"/>
+      <c r="T72" s="43"/>
+      <c r="U72" s="43"/>
+      <c r="V72" s="43"/>
+      <c r="W72" s="43"/>
+      <c r="X72" s="43"/>
+      <c r="Y72" s="48"/>
       <c r="Z72" s="1"/>
       <c r="AA72" s="1"/>
       <c r="AB72" s="1"/>

</xml_diff>

<commit_message>
[#7768] fix excel typo
</commit_message>
<xml_diff>
--- a/storage/app/excel/contact_book_0.xlsx
+++ b/storage/app/excel/contact_book_0.xlsx
@@ -145,9 +145,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -165,7 +165,36 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -173,8 +202,25 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -189,30 +235,7 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -220,29 +243,6 @@
     <font>
       <b/>
       <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -257,19 +257,34 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -281,7 +296,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -289,21 +304,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -366,25 +366,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -402,61 +438,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -474,13 +468,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -498,13 +522,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -516,37 +540,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -705,13 +705,41 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -741,21 +769,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -772,9 +785,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -787,33 +802,18 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -825,130 +825,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="17" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="16" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1488,8 +1488,8 @@
   <sheetPr/>
   <dimension ref="A1:ACU93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="N67" sqref="N67:Y73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>

</xml_diff>